<commit_message>
## 분석 시간: 2025-05-19 00:07:57
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY36"/>
+  <dimension ref="A1:AZ36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -687,6 +687,11 @@
       <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
         </is>
       </c>
     </row>
@@ -750,6 +755,7 @@
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -831,6 +837,7 @@
         </is>
       </c>
       <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -904,6 +911,7 @@
       <c r="AW4" t="inlineStr"/>
       <c r="AX4" t="inlineStr"/>
       <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -973,6 +981,7 @@
       <c r="AW5" t="inlineStr"/>
       <c r="AX5" t="inlineStr"/>
       <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1046,6 +1055,7 @@
       <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="inlineStr"/>
       <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1111,6 +1121,7 @@
       <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="inlineStr"/>
       <c r="AY7" t="inlineStr"/>
+      <c r="AZ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1184,6 +1195,7 @@
       <c r="AW8" t="inlineStr"/>
       <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1249,6 +1261,7 @@
       <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="inlineStr"/>
       <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1475,9 +1488,10 @@
       </c>
       <c r="AY10" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="AZ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1686,7 +1700,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="AY11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="AZ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1808,6 +1827,7 @@
         </is>
       </c>
       <c r="AY12" t="inlineStr"/>
+      <c r="AZ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1964,7 +1984,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="AY13" t="inlineStr"/>
+      <c r="AY13" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="AZ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2042,6 +2067,7 @@
       <c r="AW14" t="inlineStr"/>
       <c r="AX14" t="inlineStr"/>
       <c r="AY14" t="inlineStr"/>
+      <c r="AZ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2115,6 +2141,7 @@
       <c r="AW15" t="inlineStr"/>
       <c r="AX15" t="inlineStr"/>
       <c r="AY15" t="inlineStr"/>
+      <c r="AZ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2212,6 +2239,7 @@
       <c r="AW16" t="inlineStr"/>
       <c r="AX16" t="inlineStr"/>
       <c r="AY16" t="inlineStr"/>
+      <c r="AZ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2285,6 +2313,7 @@
       <c r="AW17" t="inlineStr"/>
       <c r="AX17" t="inlineStr"/>
       <c r="AY17" t="inlineStr"/>
+      <c r="AZ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2350,6 +2379,7 @@
       <c r="AW18" t="inlineStr"/>
       <c r="AX18" t="inlineStr"/>
       <c r="AY18" t="inlineStr"/>
+      <c r="AZ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2435,6 +2465,7 @@
       <c r="AW19" t="inlineStr"/>
       <c r="AX19" t="inlineStr"/>
       <c r="AY19" t="inlineStr"/>
+      <c r="AZ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2540,6 +2571,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="AZ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2605,6 +2637,7 @@
       <c r="AW21" t="inlineStr"/>
       <c r="AX21" t="inlineStr"/>
       <c r="AY21" t="inlineStr"/>
+      <c r="AZ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2674,6 +2707,7 @@
       <c r="AW22" t="inlineStr"/>
       <c r="AX22" t="inlineStr"/>
       <c r="AY22" t="inlineStr"/>
+      <c r="AZ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2760,9 +2794,10 @@
       </c>
       <c r="AY23" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="AZ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2843,7 +2878,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="AY24" t="inlineStr"/>
+      <c r="AY24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="AZ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2921,6 +2961,7 @@
       <c r="AW25" t="inlineStr"/>
       <c r="AX25" t="inlineStr"/>
       <c r="AY25" t="inlineStr"/>
+      <c r="AZ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3005,7 +3046,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="AY26" t="inlineStr"/>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="AZ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3075,6 +3121,7 @@
       <c r="AW27" t="inlineStr"/>
       <c r="AX27" t="inlineStr"/>
       <c r="AY27" t="inlineStr"/>
+      <c r="AZ27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3140,6 +3187,7 @@
       <c r="AW28" t="inlineStr"/>
       <c r="AX28" t="inlineStr"/>
       <c r="AY28" t="inlineStr"/>
+      <c r="AZ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3213,6 +3261,7 @@
       <c r="AW29" t="inlineStr"/>
       <c r="AX29" t="inlineStr"/>
       <c r="AY29" t="inlineStr"/>
+      <c r="AZ29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3282,6 +3331,7 @@
         </is>
       </c>
       <c r="AY30" t="inlineStr"/>
+      <c r="AZ30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3347,6 +3397,7 @@
       <c r="AW31" t="inlineStr"/>
       <c r="AX31" t="inlineStr"/>
       <c r="AY31" t="inlineStr"/>
+      <c r="AZ31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3412,6 +3463,7 @@
       <c r="AW32" t="inlineStr"/>
       <c r="AX32" t="inlineStr"/>
       <c r="AY32" t="inlineStr"/>
+      <c r="AZ32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3477,6 +3529,7 @@
       <c r="AW33" t="inlineStr"/>
       <c r="AX33" t="inlineStr"/>
       <c r="AY33" t="inlineStr"/>
+      <c r="AZ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3538,6 +3591,7 @@
       <c r="AW34" t="inlineStr"/>
       <c r="AX34" t="inlineStr"/>
       <c r="AY34" t="inlineStr"/>
+      <c r="AZ34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3603,6 +3657,7 @@
       </c>
       <c r="AX35" t="inlineStr"/>
       <c r="AY35" t="inlineStr"/>
+      <c r="AZ35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3671,7 +3726,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="AY36" t="inlineStr"/>
+      <c r="AY36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="AZ36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
## 분석 시간: 2025-05-22 07:47:02
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB41"/>
+  <dimension ref="A1:BC41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,6 +702,11 @@
       <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>2025-05-21</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
         </is>
       </c>
     </row>
@@ -768,6 +773,7 @@
       <c r="AZ2" t="inlineStr"/>
       <c r="BA2" t="inlineStr"/>
       <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -852,6 +858,7 @@
       <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -928,6 +935,7 @@
       <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="inlineStr"/>
       <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1000,6 +1008,7 @@
       <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="inlineStr"/>
       <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1076,6 +1085,7 @@
       <c r="AZ6" t="inlineStr"/>
       <c r="BA6" t="inlineStr"/>
       <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1144,6 +1154,7 @@
       <c r="AZ7" t="inlineStr"/>
       <c r="BA7" t="inlineStr"/>
       <c r="BB7" t="inlineStr"/>
+      <c r="BC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1220,6 +1231,7 @@
       <c r="AZ8" t="inlineStr"/>
       <c r="BA8" t="inlineStr"/>
       <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1292,6 +1304,7 @@
       </c>
       <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1531,7 +1544,16 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BB10" t="inlineStr"/>
+      <c r="BB10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BC10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1752,6 +1774,7 @@
       </c>
       <c r="BA11" t="inlineStr"/>
       <c r="BB11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1876,6 +1899,7 @@
       <c r="AZ12" t="inlineStr"/>
       <c r="BA12" t="inlineStr"/>
       <c r="BB12" t="inlineStr"/>
+      <c r="BC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2044,6 +2068,7 @@
       </c>
       <c r="BA13" t="inlineStr"/>
       <c r="BB13" t="inlineStr"/>
+      <c r="BC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2124,6 +2149,7 @@
       <c r="AZ14" t="inlineStr"/>
       <c r="BA14" t="inlineStr"/>
       <c r="BB14" t="inlineStr"/>
+      <c r="BC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2200,6 +2226,7 @@
       <c r="AZ15" t="inlineStr"/>
       <c r="BA15" t="inlineStr"/>
       <c r="BB15" t="inlineStr"/>
+      <c r="BC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2304,6 +2331,7 @@
       </c>
       <c r="BA16" t="inlineStr"/>
       <c r="BB16" t="inlineStr"/>
+      <c r="BC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2380,6 +2408,7 @@
       <c r="AZ17" t="inlineStr"/>
       <c r="BA17" t="inlineStr"/>
       <c r="BB17" t="inlineStr"/>
+      <c r="BC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2448,6 +2477,7 @@
       <c r="AZ18" t="inlineStr"/>
       <c r="BA18" t="inlineStr"/>
       <c r="BB18" t="inlineStr"/>
+      <c r="BC18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2536,6 +2566,7 @@
       <c r="AZ19" t="inlineStr"/>
       <c r="BA19" t="inlineStr"/>
       <c r="BB19" t="inlineStr"/>
+      <c r="BC19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2644,6 +2675,7 @@
       <c r="AZ20" t="inlineStr"/>
       <c r="BA20" t="inlineStr"/>
       <c r="BB20" t="inlineStr"/>
+      <c r="BC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2712,6 +2744,7 @@
       <c r="AZ21" t="inlineStr"/>
       <c r="BA21" t="inlineStr"/>
       <c r="BB21" t="inlineStr"/>
+      <c r="BC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2792,6 +2825,7 @@
         </is>
       </c>
       <c r="BB22" t="inlineStr"/>
+      <c r="BC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2887,7 +2921,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BB23" t="inlineStr"/>
+      <c r="BB23" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2979,7 +3018,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BB24" t="inlineStr"/>
+      <c r="BB24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3076,6 +3120,7 @@
       </c>
       <c r="BA25" t="inlineStr"/>
       <c r="BB25" t="inlineStr"/>
+      <c r="BC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3176,6 +3221,7 @@
         </is>
       </c>
       <c r="BB26" t="inlineStr"/>
+      <c r="BC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3256,6 +3302,7 @@
         </is>
       </c>
       <c r="BB27" t="inlineStr"/>
+      <c r="BC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3324,6 +3371,7 @@
       <c r="AZ28" t="inlineStr"/>
       <c r="BA28" t="inlineStr"/>
       <c r="BB28" t="inlineStr"/>
+      <c r="BC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3395,7 +3443,12 @@
       <c r="AY29" t="inlineStr"/>
       <c r="AZ29" t="inlineStr"/>
       <c r="BA29" t="inlineStr"/>
-      <c r="BB29" t="inlineStr"/>
+      <c r="BB29" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3468,6 +3521,7 @@
         </is>
       </c>
       <c r="BB30" t="inlineStr"/>
+      <c r="BC30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3536,6 +3590,7 @@
       <c r="AZ31" t="inlineStr"/>
       <c r="BA31" t="inlineStr"/>
       <c r="BB31" t="inlineStr"/>
+      <c r="BC31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3612,6 +3667,7 @@
         </is>
       </c>
       <c r="BB32" t="inlineStr"/>
+      <c r="BC32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3680,6 +3736,7 @@
       <c r="AZ33" t="inlineStr"/>
       <c r="BA33" t="inlineStr"/>
       <c r="BB33" t="inlineStr"/>
+      <c r="BC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3748,6 +3805,7 @@
       <c r="AZ34" t="inlineStr"/>
       <c r="BA34" t="inlineStr"/>
       <c r="BB34" t="inlineStr"/>
+      <c r="BC34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3831,7 +3889,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BB35" t="inlineStr"/>
+      <c r="BB35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3899,7 +3966,12 @@
         </is>
       </c>
       <c r="BA36" t="inlineStr"/>
-      <c r="BB36" t="inlineStr"/>
+      <c r="BB36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3971,7 +4043,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BB37" t="inlineStr"/>
+      <c r="BB37" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BC37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4040,6 +4117,7 @@
       </c>
       <c r="BA38" t="inlineStr"/>
       <c r="BB38" t="inlineStr"/>
+      <c r="BC38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4111,7 +4189,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BB39" t="inlineStr"/>
+      <c r="BB39" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BC39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4179,7 +4262,12 @@
         </is>
       </c>
       <c r="BA40" t="inlineStr"/>
-      <c r="BB40" t="inlineStr"/>
+      <c r="BB40" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BC40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4248,6 +4336,7 @@
       </c>
       <c r="BA41" t="inlineStr"/>
       <c r="BB41" t="inlineStr"/>
+      <c r="BC41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-05-24 14:23:05
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD47"/>
+  <dimension ref="A1:BE47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,6 +712,11 @@
       <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>2025-05-23</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
         </is>
       </c>
     </row>
@@ -780,6 +785,7 @@
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="inlineStr"/>
       <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -866,6 +872,7 @@
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
       <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -944,6 +951,7 @@
       <c r="BB4" t="inlineStr"/>
       <c r="BC4" t="inlineStr"/>
       <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1018,6 +1026,7 @@
       <c r="BB5" t="inlineStr"/>
       <c r="BC5" t="inlineStr"/>
       <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1096,6 +1105,7 @@
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
       <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1170,6 +1180,7 @@
         </is>
       </c>
       <c r="BD7" t="inlineStr"/>
+      <c r="BE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1248,6 +1259,7 @@
       <c r="BB8" t="inlineStr"/>
       <c r="BC8" t="inlineStr"/>
       <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1322,6 +1334,7 @@
       <c r="BB9" t="inlineStr"/>
       <c r="BC9" t="inlineStr"/>
       <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1573,6 +1586,11 @@
       </c>
       <c r="BD10" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BE10" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -1798,6 +1816,7 @@
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
       <c r="BD11" t="inlineStr"/>
+      <c r="BE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1924,6 +1943,7 @@
       <c r="BB12" t="inlineStr"/>
       <c r="BC12" t="inlineStr"/>
       <c r="BD12" t="inlineStr"/>
+      <c r="BE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2094,6 +2114,7 @@
       <c r="BB13" t="inlineStr"/>
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2176,6 +2197,7 @@
       <c r="BB14" t="inlineStr"/>
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="inlineStr"/>
+      <c r="BE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2254,6 +2276,7 @@
       <c r="BB15" t="inlineStr"/>
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
+      <c r="BE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2360,6 +2383,7 @@
       <c r="BB16" t="inlineStr"/>
       <c r="BC16" t="inlineStr"/>
       <c r="BD16" t="inlineStr"/>
+      <c r="BE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2438,6 +2462,7 @@
       <c r="BB17" t="inlineStr"/>
       <c r="BC17" t="inlineStr"/>
       <c r="BD17" t="inlineStr"/>
+      <c r="BE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2508,6 +2533,7 @@
       <c r="BB18" t="inlineStr"/>
       <c r="BC18" t="inlineStr"/>
       <c r="BD18" t="inlineStr"/>
+      <c r="BE18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2598,6 +2624,7 @@
       <c r="BB19" t="inlineStr"/>
       <c r="BC19" t="inlineStr"/>
       <c r="BD19" t="inlineStr"/>
+      <c r="BE19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2708,6 +2735,7 @@
       <c r="BB20" t="inlineStr"/>
       <c r="BC20" t="inlineStr"/>
       <c r="BD20" t="inlineStr"/>
+      <c r="BE20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2778,6 +2806,7 @@
       <c r="BB21" t="inlineStr"/>
       <c r="BC21" t="inlineStr"/>
       <c r="BD21" t="inlineStr"/>
+      <c r="BE21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2864,6 +2893,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BE22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2970,6 +3000,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BE23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3068,6 +3099,7 @@
       </c>
       <c r="BC24" t="inlineStr"/>
       <c r="BD24" t="inlineStr"/>
+      <c r="BE24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3166,6 +3198,7 @@
       <c r="BB25" t="inlineStr"/>
       <c r="BC25" t="inlineStr"/>
       <c r="BD25" t="inlineStr"/>
+      <c r="BE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3272,6 +3305,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BE26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3354,6 +3388,7 @@
       <c r="BB27" t="inlineStr"/>
       <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
+      <c r="BE27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3424,6 +3459,7 @@
       <c r="BB28" t="inlineStr"/>
       <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
+      <c r="BE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3502,6 +3538,7 @@
       </c>
       <c r="BC29" t="inlineStr"/>
       <c r="BD29" t="inlineStr"/>
+      <c r="BE29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3576,6 +3613,7 @@
       <c r="BB30" t="inlineStr"/>
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
+      <c r="BE30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3646,6 +3684,7 @@
       <c r="BB31" t="inlineStr"/>
       <c r="BC31" t="inlineStr"/>
       <c r="BD31" t="inlineStr"/>
+      <c r="BE31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3724,6 +3763,7 @@
       <c r="BB32" t="inlineStr"/>
       <c r="BC32" t="inlineStr"/>
       <c r="BD32" t="inlineStr"/>
+      <c r="BE32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3794,6 +3834,7 @@
       <c r="BB33" t="inlineStr"/>
       <c r="BC33" t="inlineStr"/>
       <c r="BD33" t="inlineStr"/>
+      <c r="BE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3864,6 +3905,7 @@
       <c r="BB34" t="inlineStr"/>
       <c r="BC34" t="inlineStr"/>
       <c r="BD34" t="inlineStr"/>
+      <c r="BE34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3958,6 +4000,7 @@
         </is>
       </c>
       <c r="BD35" t="inlineStr"/>
+      <c r="BE35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4031,7 +4074,12 @@
         </is>
       </c>
       <c r="BC36" t="inlineStr"/>
-      <c r="BD36" t="inlineStr"/>
+      <c r="BD36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BE36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4113,7 +4161,16 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BD37" t="inlineStr"/>
+      <c r="BD37" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BE37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4184,6 +4241,7 @@
       <c r="BB38" t="inlineStr"/>
       <c r="BC38" t="inlineStr"/>
       <c r="BD38" t="inlineStr"/>
+      <c r="BE38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4267,9 +4325,10 @@
       </c>
       <c r="BD39" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BE39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4348,6 +4407,7 @@
         </is>
       </c>
       <c r="BD40" t="inlineStr"/>
+      <c r="BE40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4418,6 +4478,7 @@
       <c r="BB41" t="inlineStr"/>
       <c r="BC41" t="inlineStr"/>
       <c r="BD41" t="inlineStr"/>
+      <c r="BE41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4489,6 +4550,11 @@
       </c>
       <c r="BD42" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BE42" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -4562,6 +4628,7 @@
         </is>
       </c>
       <c r="BD43" t="inlineStr"/>
+      <c r="BE43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4636,6 +4703,11 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BE44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4706,6 +4778,11 @@
         </is>
       </c>
       <c r="BD45" t="inlineStr"/>
+      <c r="BE45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4776,6 +4853,7 @@
         </is>
       </c>
       <c r="BD46" t="inlineStr"/>
+      <c r="BE46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4846,6 +4924,7 @@
         </is>
       </c>
       <c r="BD47" t="inlineStr"/>
+      <c r="BE47" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
## 분석 시간: 2025-05-25 09:03:37
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BE47"/>
+  <dimension ref="A1:BF47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,6 +717,11 @@
       <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>2025-05-24</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-25</t>
         </is>
       </c>
     </row>
@@ -786,6 +791,7 @@
       <c r="BC2" t="inlineStr"/>
       <c r="BD2" t="inlineStr"/>
       <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -873,6 +879,7 @@
       <c r="BC3" t="inlineStr"/>
       <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -952,6 +959,7 @@
       <c r="BC4" t="inlineStr"/>
       <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1027,6 +1035,7 @@
       <c r="BC5" t="inlineStr"/>
       <c r="BD5" t="inlineStr"/>
       <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1106,6 +1115,7 @@
       <c r="BC6" t="inlineStr"/>
       <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
+      <c r="BF6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1181,6 +1191,7 @@
       </c>
       <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="inlineStr"/>
+      <c r="BF7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1260,6 +1271,7 @@
       <c r="BC8" t="inlineStr"/>
       <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
+      <c r="BF8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1335,6 +1347,7 @@
       <c r="BC9" t="inlineStr"/>
       <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
+      <c r="BF9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1591,9 +1604,10 @@
       </c>
       <c r="BE10" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BF10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1816,7 +1830,12 @@
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
       <c r="BD11" t="inlineStr"/>
-      <c r="BE11" t="inlineStr"/>
+      <c r="BE11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1943,7 +1962,12 @@
       <c r="BB12" t="inlineStr"/>
       <c r="BC12" t="inlineStr"/>
       <c r="BD12" t="inlineStr"/>
-      <c r="BE12" t="inlineStr"/>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2115,6 +2139,7 @@
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="inlineStr"/>
+      <c r="BF13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2198,6 +2223,7 @@
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="inlineStr"/>
       <c r="BE14" t="inlineStr"/>
+      <c r="BF14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2277,6 +2303,7 @@
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
       <c r="BE15" t="inlineStr"/>
+      <c r="BF15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2384,6 +2411,7 @@
       <c r="BC16" t="inlineStr"/>
       <c r="BD16" t="inlineStr"/>
       <c r="BE16" t="inlineStr"/>
+      <c r="BF16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2463,6 +2491,7 @@
       <c r="BC17" t="inlineStr"/>
       <c r="BD17" t="inlineStr"/>
       <c r="BE17" t="inlineStr"/>
+      <c r="BF17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2534,6 +2563,7 @@
       <c r="BC18" t="inlineStr"/>
       <c r="BD18" t="inlineStr"/>
       <c r="BE18" t="inlineStr"/>
+      <c r="BF18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2625,6 +2655,7 @@
       <c r="BC19" t="inlineStr"/>
       <c r="BD19" t="inlineStr"/>
       <c r="BE19" t="inlineStr"/>
+      <c r="BF19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2735,7 +2766,12 @@
       <c r="BB20" t="inlineStr"/>
       <c r="BC20" t="inlineStr"/>
       <c r="BD20" t="inlineStr"/>
-      <c r="BE20" t="inlineStr"/>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BF20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2807,6 +2843,7 @@
       <c r="BC21" t="inlineStr"/>
       <c r="BD21" t="inlineStr"/>
       <c r="BE21" t="inlineStr"/>
+      <c r="BF21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2894,6 +2931,7 @@
         </is>
       </c>
       <c r="BE22" t="inlineStr"/>
+      <c r="BF22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3001,6 +3039,7 @@
         </is>
       </c>
       <c r="BE23" t="inlineStr"/>
+      <c r="BF23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3099,7 +3138,12 @@
       </c>
       <c r="BC24" t="inlineStr"/>
       <c r="BD24" t="inlineStr"/>
-      <c r="BE24" t="inlineStr"/>
+      <c r="BE24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3199,6 +3243,7 @@
       <c r="BC25" t="inlineStr"/>
       <c r="BD25" t="inlineStr"/>
       <c r="BE25" t="inlineStr"/>
+      <c r="BF25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3306,6 +3351,7 @@
         </is>
       </c>
       <c r="BE26" t="inlineStr"/>
+      <c r="BF26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3389,6 +3435,7 @@
       <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
       <c r="BE27" t="inlineStr"/>
+      <c r="BF27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3460,6 +3507,7 @@
       <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
       <c r="BE28" t="inlineStr"/>
+      <c r="BF28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3539,6 +3587,7 @@
       <c r="BC29" t="inlineStr"/>
       <c r="BD29" t="inlineStr"/>
       <c r="BE29" t="inlineStr"/>
+      <c r="BF29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3614,6 +3663,7 @@
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
       <c r="BE30" t="inlineStr"/>
+      <c r="BF30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3685,6 +3735,7 @@
       <c r="BC31" t="inlineStr"/>
       <c r="BD31" t="inlineStr"/>
       <c r="BE31" t="inlineStr"/>
+      <c r="BF31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3764,6 +3815,7 @@
       <c r="BC32" t="inlineStr"/>
       <c r="BD32" t="inlineStr"/>
       <c r="BE32" t="inlineStr"/>
+      <c r="BF32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3835,6 +3887,7 @@
       <c r="BC33" t="inlineStr"/>
       <c r="BD33" t="inlineStr"/>
       <c r="BE33" t="inlineStr"/>
+      <c r="BF33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3906,6 +3959,7 @@
       <c r="BC34" t="inlineStr"/>
       <c r="BD34" t="inlineStr"/>
       <c r="BE34" t="inlineStr"/>
+      <c r="BF34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4000,7 +4054,12 @@
         </is>
       </c>
       <c r="BD35" t="inlineStr"/>
-      <c r="BE35" t="inlineStr"/>
+      <c r="BE35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4080,6 +4139,7 @@
         </is>
       </c>
       <c r="BE36" t="inlineStr"/>
+      <c r="BF36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4168,9 +4228,10 @@
       </c>
       <c r="BE37" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BF37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4242,6 +4303,7 @@
       <c r="BC38" t="inlineStr"/>
       <c r="BD38" t="inlineStr"/>
       <c r="BE38" t="inlineStr"/>
+      <c r="BF38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4328,7 +4390,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BE39" t="inlineStr"/>
+      <c r="BE39" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4408,6 +4475,7 @@
       </c>
       <c r="BD40" t="inlineStr"/>
       <c r="BE40" t="inlineStr"/>
+      <c r="BF40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4478,7 +4546,12 @@
       <c r="BB41" t="inlineStr"/>
       <c r="BC41" t="inlineStr"/>
       <c r="BD41" t="inlineStr"/>
-      <c r="BE41" t="inlineStr"/>
+      <c r="BE41" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BF41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4555,9 +4628,10 @@
       </c>
       <c r="BE42" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BF42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4627,8 +4701,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BD43" t="inlineStr"/>
-      <c r="BE43" t="inlineStr"/>
+      <c r="BD43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BE43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4708,6 +4791,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BF44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4783,6 +4867,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BF45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4854,6 +4939,7 @@
       </c>
       <c r="BD46" t="inlineStr"/>
       <c r="BE46" t="inlineStr"/>
+      <c r="BF46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4923,8 +5009,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BD47" t="inlineStr"/>
-      <c r="BE47" t="inlineStr"/>
+      <c r="BD47" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BE47" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BF47" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-05-26 08:50:43
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF47"/>
+  <dimension ref="A1:BG47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,6 +722,11 @@
       <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>2025-05-25</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
         </is>
       </c>
     </row>
@@ -792,6 +797,7 @@
       <c r="BD2" t="inlineStr"/>
       <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -880,6 +886,11 @@
       <c r="BD3" t="inlineStr"/>
       <c r="BE3" t="inlineStr"/>
       <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -960,6 +971,7 @@
       <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1036,6 +1048,7 @@
       <c r="BD5" t="inlineStr"/>
       <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1116,6 +1129,7 @@
       <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
+      <c r="BG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1192,6 +1206,7 @@
       <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="inlineStr"/>
       <c r="BF7" t="inlineStr"/>
+      <c r="BG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1272,6 +1287,7 @@
       <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
       <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1348,6 +1364,7 @@
       <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
       <c r="BF9" t="inlineStr"/>
+      <c r="BG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1607,7 +1624,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BF10" t="inlineStr"/>
+      <c r="BF10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1836,6 +1858,7 @@
         </is>
       </c>
       <c r="BF11" t="inlineStr"/>
+      <c r="BG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1968,6 +1991,7 @@
         </is>
       </c>
       <c r="BF12" t="inlineStr"/>
+      <c r="BG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2140,6 +2164,7 @@
       <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="inlineStr"/>
       <c r="BF13" t="inlineStr"/>
+      <c r="BG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2224,6 +2249,7 @@
       <c r="BD14" t="inlineStr"/>
       <c r="BE14" t="inlineStr"/>
       <c r="BF14" t="inlineStr"/>
+      <c r="BG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2304,6 +2330,7 @@
       <c r="BD15" t="inlineStr"/>
       <c r="BE15" t="inlineStr"/>
       <c r="BF15" t="inlineStr"/>
+      <c r="BG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2412,6 +2439,7 @@
       <c r="BD16" t="inlineStr"/>
       <c r="BE16" t="inlineStr"/>
       <c r="BF16" t="inlineStr"/>
+      <c r="BG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2492,6 +2520,7 @@
       <c r="BD17" t="inlineStr"/>
       <c r="BE17" t="inlineStr"/>
       <c r="BF17" t="inlineStr"/>
+      <c r="BG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2564,6 +2593,7 @@
       <c r="BD18" t="inlineStr"/>
       <c r="BE18" t="inlineStr"/>
       <c r="BF18" t="inlineStr"/>
+      <c r="BG18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2656,6 +2686,7 @@
       <c r="BD19" t="inlineStr"/>
       <c r="BE19" t="inlineStr"/>
       <c r="BF19" t="inlineStr"/>
+      <c r="BG19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2772,6 +2803,7 @@
         </is>
       </c>
       <c r="BF20" t="inlineStr"/>
+      <c r="BG20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2844,6 +2876,7 @@
       <c r="BD21" t="inlineStr"/>
       <c r="BE21" t="inlineStr"/>
       <c r="BF21" t="inlineStr"/>
+      <c r="BG21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2932,6 +2965,7 @@
       </c>
       <c r="BE22" t="inlineStr"/>
       <c r="BF22" t="inlineStr"/>
+      <c r="BG22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3039,7 +3073,12 @@
         </is>
       </c>
       <c r="BE23" t="inlineStr"/>
-      <c r="BF23" t="inlineStr"/>
+      <c r="BF23" t="inlineStr">
+        <is>
+          <t>대화 (58.0kg)</t>
+        </is>
+      </c>
+      <c r="BG23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3144,6 +3183,7 @@
         </is>
       </c>
       <c r="BF24" t="inlineStr"/>
+      <c r="BG24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3244,6 +3284,7 @@
       <c r="BD25" t="inlineStr"/>
       <c r="BE25" t="inlineStr"/>
       <c r="BF25" t="inlineStr"/>
+      <c r="BG25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3352,6 +3393,7 @@
       </c>
       <c r="BE26" t="inlineStr"/>
       <c r="BF26" t="inlineStr"/>
+      <c r="BG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3436,6 +3478,7 @@
       <c r="BD27" t="inlineStr"/>
       <c r="BE27" t="inlineStr"/>
       <c r="BF27" t="inlineStr"/>
+      <c r="BG27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3508,6 +3551,7 @@
       <c r="BD28" t="inlineStr"/>
       <c r="BE28" t="inlineStr"/>
       <c r="BF28" t="inlineStr"/>
+      <c r="BG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3588,6 +3632,7 @@
       <c r="BD29" t="inlineStr"/>
       <c r="BE29" t="inlineStr"/>
       <c r="BF29" t="inlineStr"/>
+      <c r="BG29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3664,6 +3709,7 @@
       <c r="BD30" t="inlineStr"/>
       <c r="BE30" t="inlineStr"/>
       <c r="BF30" t="inlineStr"/>
+      <c r="BG30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3736,6 +3782,7 @@
       <c r="BD31" t="inlineStr"/>
       <c r="BE31" t="inlineStr"/>
       <c r="BF31" t="inlineStr"/>
+      <c r="BG31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3816,6 +3863,7 @@
       <c r="BD32" t="inlineStr"/>
       <c r="BE32" t="inlineStr"/>
       <c r="BF32" t="inlineStr"/>
+      <c r="BG32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3888,6 +3936,7 @@
       <c r="BD33" t="inlineStr"/>
       <c r="BE33" t="inlineStr"/>
       <c r="BF33" t="inlineStr"/>
+      <c r="BG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3960,6 +4009,7 @@
       <c r="BD34" t="inlineStr"/>
       <c r="BE34" t="inlineStr"/>
       <c r="BF34" t="inlineStr"/>
+      <c r="BG34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4059,7 +4109,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BF35" t="inlineStr"/>
+      <c r="BF35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4139,7 +4194,12 @@
         </is>
       </c>
       <c r="BE36" t="inlineStr"/>
-      <c r="BF36" t="inlineStr"/>
+      <c r="BF36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4231,7 +4291,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BF37" t="inlineStr"/>
+      <c r="BF37" t="inlineStr">
+        <is>
+          <t>대화 (78.9kg)</t>
+        </is>
+      </c>
+      <c r="BG37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4304,6 +4369,7 @@
       <c r="BD38" t="inlineStr"/>
       <c r="BE38" t="inlineStr"/>
       <c r="BF38" t="inlineStr"/>
+      <c r="BG38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4395,7 +4461,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BF39" t="inlineStr"/>
+      <c r="BF39" t="inlineStr">
+        <is>
+          <t>대화 (104.9kg)</t>
+        </is>
+      </c>
+      <c r="BG39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4475,7 +4546,12 @@
       </c>
       <c r="BD40" t="inlineStr"/>
       <c r="BE40" t="inlineStr"/>
-      <c r="BF40" t="inlineStr"/>
+      <c r="BF40" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4551,7 +4627,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BF41" t="inlineStr"/>
+      <c r="BF41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4631,7 +4712,16 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BF42" t="inlineStr"/>
+      <c r="BF42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4711,7 +4801,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BF43" t="inlineStr"/>
+      <c r="BF43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4791,7 +4886,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BF44" t="inlineStr"/>
+      <c r="BF44" t="inlineStr">
+        <is>
+          <t>대화 (88.4kg)</t>
+        </is>
+      </c>
+      <c r="BG44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4867,7 +4967,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BF45" t="inlineStr"/>
+      <c r="BF45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BG45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4940,6 +5045,7 @@
       <c r="BD46" t="inlineStr"/>
       <c r="BE46" t="inlineStr"/>
       <c r="BF46" t="inlineStr"/>
+      <c r="BG46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5020,6 +5126,7 @@
         </is>
       </c>
       <c r="BF47" t="inlineStr"/>
+      <c r="BG47" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-05-27 00:42:58
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG47"/>
+  <dimension ref="A1:BH48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,6 +727,11 @@
       <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>2025-05-26</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
         </is>
       </c>
     </row>
@@ -798,6 +803,7 @@
       <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="inlineStr"/>
       <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -891,6 +897,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BH3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -972,6 +979,7 @@
       <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
       <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1049,6 +1057,7 @@
       <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="inlineStr"/>
       <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1130,6 +1139,7 @@
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
       <c r="BG6" t="inlineStr"/>
+      <c r="BH6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1207,6 +1217,7 @@
       <c r="BE7" t="inlineStr"/>
       <c r="BF7" t="inlineStr"/>
       <c r="BG7" t="inlineStr"/>
+      <c r="BH7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1288,6 +1299,7 @@
       <c r="BE8" t="inlineStr"/>
       <c r="BF8" t="inlineStr"/>
       <c r="BG8" t="inlineStr"/>
+      <c r="BH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1365,6 +1377,7 @@
       <c r="BE9" t="inlineStr"/>
       <c r="BF9" t="inlineStr"/>
       <c r="BG9" t="inlineStr"/>
+      <c r="BH9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1630,6 +1643,7 @@
         </is>
       </c>
       <c r="BG10" t="inlineStr"/>
+      <c r="BH10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1859,6 +1873,7 @@
       </c>
       <c r="BF11" t="inlineStr"/>
       <c r="BG11" t="inlineStr"/>
+      <c r="BH11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1992,6 +2007,7 @@
       </c>
       <c r="BF12" t="inlineStr"/>
       <c r="BG12" t="inlineStr"/>
+      <c r="BH12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2165,6 +2181,7 @@
       <c r="BE13" t="inlineStr"/>
       <c r="BF13" t="inlineStr"/>
       <c r="BG13" t="inlineStr"/>
+      <c r="BH13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2250,6 +2267,7 @@
       <c r="BE14" t="inlineStr"/>
       <c r="BF14" t="inlineStr"/>
       <c r="BG14" t="inlineStr"/>
+      <c r="BH14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2331,6 +2349,7 @@
       <c r="BE15" t="inlineStr"/>
       <c r="BF15" t="inlineStr"/>
       <c r="BG15" t="inlineStr"/>
+      <c r="BH15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2440,6 +2459,7 @@
       <c r="BE16" t="inlineStr"/>
       <c r="BF16" t="inlineStr"/>
       <c r="BG16" t="inlineStr"/>
+      <c r="BH16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2521,6 +2541,7 @@
       <c r="BE17" t="inlineStr"/>
       <c r="BF17" t="inlineStr"/>
       <c r="BG17" t="inlineStr"/>
+      <c r="BH17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2594,6 +2615,7 @@
       <c r="BE18" t="inlineStr"/>
       <c r="BF18" t="inlineStr"/>
       <c r="BG18" t="inlineStr"/>
+      <c r="BH18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2687,6 +2709,7 @@
       <c r="BE19" t="inlineStr"/>
       <c r="BF19" t="inlineStr"/>
       <c r="BG19" t="inlineStr"/>
+      <c r="BH19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2804,6 +2827,7 @@
       </c>
       <c r="BF20" t="inlineStr"/>
       <c r="BG20" t="inlineStr"/>
+      <c r="BH20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2877,6 +2901,7 @@
       <c r="BE21" t="inlineStr"/>
       <c r="BF21" t="inlineStr"/>
       <c r="BG21" t="inlineStr"/>
+      <c r="BH21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2966,6 +2991,7 @@
       <c r="BE22" t="inlineStr"/>
       <c r="BF22" t="inlineStr"/>
       <c r="BG22" t="inlineStr"/>
+      <c r="BH22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3079,6 +3105,7 @@
         </is>
       </c>
       <c r="BG23" t="inlineStr"/>
+      <c r="BH23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3184,6 +3211,7 @@
       </c>
       <c r="BF24" t="inlineStr"/>
       <c r="BG24" t="inlineStr"/>
+      <c r="BH24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3285,6 +3313,7 @@
       <c r="BE25" t="inlineStr"/>
       <c r="BF25" t="inlineStr"/>
       <c r="BG25" t="inlineStr"/>
+      <c r="BH25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3394,6 +3423,7 @@
       <c r="BE26" t="inlineStr"/>
       <c r="BF26" t="inlineStr"/>
       <c r="BG26" t="inlineStr"/>
+      <c r="BH26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3479,6 +3509,7 @@
       <c r="BE27" t="inlineStr"/>
       <c r="BF27" t="inlineStr"/>
       <c r="BG27" t="inlineStr"/>
+      <c r="BH27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3552,6 +3583,7 @@
       <c r="BE28" t="inlineStr"/>
       <c r="BF28" t="inlineStr"/>
       <c r="BG28" t="inlineStr"/>
+      <c r="BH28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3633,6 +3665,7 @@
       <c r="BE29" t="inlineStr"/>
       <c r="BF29" t="inlineStr"/>
       <c r="BG29" t="inlineStr"/>
+      <c r="BH29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3710,6 +3743,7 @@
       <c r="BE30" t="inlineStr"/>
       <c r="BF30" t="inlineStr"/>
       <c r="BG30" t="inlineStr"/>
+      <c r="BH30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3783,6 +3817,7 @@
       <c r="BE31" t="inlineStr"/>
       <c r="BF31" t="inlineStr"/>
       <c r="BG31" t="inlineStr"/>
+      <c r="BH31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3864,6 +3899,7 @@
       <c r="BE32" t="inlineStr"/>
       <c r="BF32" t="inlineStr"/>
       <c r="BG32" t="inlineStr"/>
+      <c r="BH32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3937,6 +3973,7 @@
       <c r="BE33" t="inlineStr"/>
       <c r="BF33" t="inlineStr"/>
       <c r="BG33" t="inlineStr"/>
+      <c r="BH33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4010,6 +4047,7 @@
       <c r="BE34" t="inlineStr"/>
       <c r="BF34" t="inlineStr"/>
       <c r="BG34" t="inlineStr"/>
+      <c r="BH34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4114,7 +4152,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BG35" t="inlineStr"/>
+      <c r="BG35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4200,6 +4243,7 @@
         </is>
       </c>
       <c r="BG36" t="inlineStr"/>
+      <c r="BH36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4296,7 +4340,12 @@
           <t>대화 (78.9kg)</t>
         </is>
       </c>
-      <c r="BG37" t="inlineStr"/>
+      <c r="BG37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4370,6 +4419,7 @@
       <c r="BE38" t="inlineStr"/>
       <c r="BF38" t="inlineStr"/>
       <c r="BG38" t="inlineStr"/>
+      <c r="BH38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4466,7 +4516,12 @@
           <t>대화 (104.9kg)</t>
         </is>
       </c>
-      <c r="BG39" t="inlineStr"/>
+      <c r="BG39" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4552,6 +4607,7 @@
         </is>
       </c>
       <c r="BG40" t="inlineStr"/>
+      <c r="BH40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4633,6 +4689,7 @@
         </is>
       </c>
       <c r="BG41" t="inlineStr"/>
+      <c r="BH41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4719,9 +4776,10 @@
       </c>
       <c r="BG42" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BH42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4806,7 +4864,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BG43" t="inlineStr"/>
+      <c r="BG43" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BH43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4891,7 +4954,12 @@
           <t>대화 (88.4kg)</t>
         </is>
       </c>
-      <c r="BG44" t="inlineStr"/>
+      <c r="BG44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4972,7 +5040,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BG45" t="inlineStr"/>
+      <c r="BG45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5046,6 +5119,7 @@
       <c r="BE46" t="inlineStr"/>
       <c r="BF46" t="inlineStr"/>
       <c r="BG46" t="inlineStr"/>
+      <c r="BH46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5127,6 +5201,77 @@
       </c>
       <c r="BF47" t="inlineStr"/>
       <c r="BG47" t="inlineStr"/>
+      <c r="BH47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>gpqk1009</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
+      <c r="AA48" t="inlineStr"/>
+      <c r="AB48" t="inlineStr"/>
+      <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
+      <c r="AI48" t="inlineStr"/>
+      <c r="AJ48" t="inlineStr"/>
+      <c r="AK48" t="inlineStr"/>
+      <c r="AL48" t="inlineStr"/>
+      <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr"/>
+      <c r="AO48" t="inlineStr"/>
+      <c r="AP48" t="inlineStr"/>
+      <c r="AQ48" t="inlineStr"/>
+      <c r="AR48" t="inlineStr"/>
+      <c r="AS48" t="inlineStr"/>
+      <c r="AT48" t="inlineStr"/>
+      <c r="AU48" t="inlineStr"/>
+      <c r="AV48" t="inlineStr"/>
+      <c r="AW48" t="inlineStr"/>
+      <c r="AX48" t="inlineStr"/>
+      <c r="AY48" t="inlineStr"/>
+      <c r="AZ48" t="inlineStr"/>
+      <c r="BA48" t="inlineStr"/>
+      <c r="BB48" t="inlineStr"/>
+      <c r="BC48" t="inlineStr"/>
+      <c r="BD48" t="inlineStr"/>
+      <c r="BE48" t="inlineStr"/>
+      <c r="BF48" t="inlineStr"/>
+      <c r="BG48" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-05-28 13:23:36
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH48"/>
+  <dimension ref="A1:BI48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,6 +732,11 @@
       <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>2025-05-27</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -804,6 +809,7 @@
       <c r="BF2" t="inlineStr"/>
       <c r="BG2" t="inlineStr"/>
       <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -898,6 +904,7 @@
         </is>
       </c>
       <c r="BH3" t="inlineStr"/>
+      <c r="BI3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -980,6 +987,7 @@
       <c r="BF4" t="inlineStr"/>
       <c r="BG4" t="inlineStr"/>
       <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1058,6 +1066,7 @@
       <c r="BF5" t="inlineStr"/>
       <c r="BG5" t="inlineStr"/>
       <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1140,6 +1149,7 @@
       <c r="BF6" t="inlineStr"/>
       <c r="BG6" t="inlineStr"/>
       <c r="BH6" t="inlineStr"/>
+      <c r="BI6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1218,6 +1228,7 @@
       <c r="BF7" t="inlineStr"/>
       <c r="BG7" t="inlineStr"/>
       <c r="BH7" t="inlineStr"/>
+      <c r="BI7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1300,6 +1311,7 @@
       <c r="BF8" t="inlineStr"/>
       <c r="BG8" t="inlineStr"/>
       <c r="BH8" t="inlineStr"/>
+      <c r="BI8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1378,6 +1390,7 @@
       <c r="BF9" t="inlineStr"/>
       <c r="BG9" t="inlineStr"/>
       <c r="BH9" t="inlineStr"/>
+      <c r="BI9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1643,7 +1656,16 @@
         </is>
       </c>
       <c r="BG10" t="inlineStr"/>
-      <c r="BH10" t="inlineStr"/>
+      <c r="BH10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BI10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1873,7 +1895,12 @@
       </c>
       <c r="BF11" t="inlineStr"/>
       <c r="BG11" t="inlineStr"/>
-      <c r="BH11" t="inlineStr"/>
+      <c r="BH11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2006,8 +2033,17 @@
         </is>
       </c>
       <c r="BF12" t="inlineStr"/>
-      <c r="BG12" t="inlineStr"/>
-      <c r="BH12" t="inlineStr"/>
+      <c r="BG12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2182,6 +2218,7 @@
       <c r="BF13" t="inlineStr"/>
       <c r="BG13" t="inlineStr"/>
       <c r="BH13" t="inlineStr"/>
+      <c r="BI13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2268,6 +2305,7 @@
       <c r="BF14" t="inlineStr"/>
       <c r="BG14" t="inlineStr"/>
       <c r="BH14" t="inlineStr"/>
+      <c r="BI14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2350,6 +2388,7 @@
       <c r="BF15" t="inlineStr"/>
       <c r="BG15" t="inlineStr"/>
       <c r="BH15" t="inlineStr"/>
+      <c r="BI15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2460,6 +2499,7 @@
       <c r="BF16" t="inlineStr"/>
       <c r="BG16" t="inlineStr"/>
       <c r="BH16" t="inlineStr"/>
+      <c r="BI16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2542,6 +2582,7 @@
       <c r="BF17" t="inlineStr"/>
       <c r="BG17" t="inlineStr"/>
       <c r="BH17" t="inlineStr"/>
+      <c r="BI17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2616,6 +2657,7 @@
       <c r="BF18" t="inlineStr"/>
       <c r="BG18" t="inlineStr"/>
       <c r="BH18" t="inlineStr"/>
+      <c r="BI18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2710,6 +2752,11 @@
       <c r="BF19" t="inlineStr"/>
       <c r="BG19" t="inlineStr"/>
       <c r="BH19" t="inlineStr"/>
+      <c r="BI19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2827,7 +2874,12 @@
       </c>
       <c r="BF20" t="inlineStr"/>
       <c r="BG20" t="inlineStr"/>
-      <c r="BH20" t="inlineStr"/>
+      <c r="BH20" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2902,6 +2954,7 @@
       <c r="BF21" t="inlineStr"/>
       <c r="BG21" t="inlineStr"/>
       <c r="BH21" t="inlineStr"/>
+      <c r="BI21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2991,7 +3044,12 @@
       <c r="BE22" t="inlineStr"/>
       <c r="BF22" t="inlineStr"/>
       <c r="BG22" t="inlineStr"/>
-      <c r="BH22" t="inlineStr"/>
+      <c r="BH22" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3106,6 +3164,7 @@
       </c>
       <c r="BG23" t="inlineStr"/>
       <c r="BH23" t="inlineStr"/>
+      <c r="BI23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3212,6 +3271,7 @@
       <c r="BF24" t="inlineStr"/>
       <c r="BG24" t="inlineStr"/>
       <c r="BH24" t="inlineStr"/>
+      <c r="BI24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3314,6 +3374,7 @@
       <c r="BF25" t="inlineStr"/>
       <c r="BG25" t="inlineStr"/>
       <c r="BH25" t="inlineStr"/>
+      <c r="BI25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3424,6 +3485,7 @@
       <c r="BF26" t="inlineStr"/>
       <c r="BG26" t="inlineStr"/>
       <c r="BH26" t="inlineStr"/>
+      <c r="BI26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3510,6 +3572,7 @@
       <c r="BF27" t="inlineStr"/>
       <c r="BG27" t="inlineStr"/>
       <c r="BH27" t="inlineStr"/>
+      <c r="BI27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3584,6 +3647,7 @@
       <c r="BF28" t="inlineStr"/>
       <c r="BG28" t="inlineStr"/>
       <c r="BH28" t="inlineStr"/>
+      <c r="BI28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3665,7 +3729,12 @@
       <c r="BE29" t="inlineStr"/>
       <c r="BF29" t="inlineStr"/>
       <c r="BG29" t="inlineStr"/>
-      <c r="BH29" t="inlineStr"/>
+      <c r="BH29" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3743,7 +3812,12 @@
       <c r="BE30" t="inlineStr"/>
       <c r="BF30" t="inlineStr"/>
       <c r="BG30" t="inlineStr"/>
-      <c r="BH30" t="inlineStr"/>
+      <c r="BH30" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3818,6 +3892,7 @@
       <c r="BF31" t="inlineStr"/>
       <c r="BG31" t="inlineStr"/>
       <c r="BH31" t="inlineStr"/>
+      <c r="BI31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3899,7 +3974,16 @@
       <c r="BE32" t="inlineStr"/>
       <c r="BF32" t="inlineStr"/>
       <c r="BG32" t="inlineStr"/>
-      <c r="BH32" t="inlineStr"/>
+      <c r="BH32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3974,6 +4058,7 @@
       <c r="BF33" t="inlineStr"/>
       <c r="BG33" t="inlineStr"/>
       <c r="BH33" t="inlineStr"/>
+      <c r="BI33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4048,6 +4133,7 @@
       <c r="BF34" t="inlineStr"/>
       <c r="BG34" t="inlineStr"/>
       <c r="BH34" t="inlineStr"/>
+      <c r="BI34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4157,7 +4243,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BH35" t="inlineStr"/>
+      <c r="BH35" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BI35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4224,7 +4315,11 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BA36" t="inlineStr"/>
+      <c r="BA36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
       <c r="BB36" t="inlineStr">
         <is>
           <t>식단</t>
@@ -4236,14 +4331,27 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BE36" t="inlineStr"/>
+      <c r="BE36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
       <c r="BF36" t="inlineStr">
         <is>
           <t>식단</t>
         </is>
       </c>
-      <c r="BG36" t="inlineStr"/>
-      <c r="BH36" t="inlineStr"/>
+      <c r="BG36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BH36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4346,6 +4454,7 @@
         </is>
       </c>
       <c r="BH37" t="inlineStr"/>
+      <c r="BI37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4420,6 +4529,7 @@
       <c r="BF38" t="inlineStr"/>
       <c r="BG38" t="inlineStr"/>
       <c r="BH38" t="inlineStr"/>
+      <c r="BI38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4522,6 +4632,7 @@
         </is>
       </c>
       <c r="BH39" t="inlineStr"/>
+      <c r="BI39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4607,7 +4718,12 @@
         </is>
       </c>
       <c r="BG40" t="inlineStr"/>
-      <c r="BH40" t="inlineStr"/>
+      <c r="BH40" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4690,6 +4806,7 @@
       </c>
       <c r="BG41" t="inlineStr"/>
       <c r="BH41" t="inlineStr"/>
+      <c r="BI41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4779,7 +4896,16 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BH42" t="inlineStr"/>
+      <c r="BH42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4869,7 +4995,16 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BH43" t="inlineStr"/>
+      <c r="BH43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4959,7 +5094,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BH44" t="inlineStr"/>
+      <c r="BH44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5045,7 +5185,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BH45" t="inlineStr"/>
+      <c r="BH45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5120,6 +5269,7 @@
       <c r="BF46" t="inlineStr"/>
       <c r="BG46" t="inlineStr"/>
       <c r="BH46" t="inlineStr"/>
+      <c r="BI46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5202,9 +5352,14 @@
       <c r="BF47" t="inlineStr"/>
       <c r="BG47" t="inlineStr"/>
       <c r="BH47" t="inlineStr"/>
+      <c r="BI47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>이정헌</t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>gpqk1009</t>
@@ -5272,6 +5427,7 @@
         </is>
       </c>
       <c r="BH48" t="inlineStr"/>
+      <c r="BI48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-05-29 09:45:17
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI48"/>
+  <dimension ref="A1:BJ48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -737,6 +737,11 @@
       <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>2025-05-28</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
         </is>
       </c>
     </row>
@@ -810,6 +815,7 @@
       <c r="BG2" t="inlineStr"/>
       <c r="BH2" t="inlineStr"/>
       <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -905,6 +911,7 @@
       </c>
       <c r="BH3" t="inlineStr"/>
       <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -988,6 +995,7 @@
       <c r="BG4" t="inlineStr"/>
       <c r="BH4" t="inlineStr"/>
       <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1067,6 +1075,7 @@
       <c r="BG5" t="inlineStr"/>
       <c r="BH5" t="inlineStr"/>
       <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1150,6 +1159,7 @@
       <c r="BG6" t="inlineStr"/>
       <c r="BH6" t="inlineStr"/>
       <c r="BI6" t="inlineStr"/>
+      <c r="BJ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1229,6 +1239,7 @@
       <c r="BG7" t="inlineStr"/>
       <c r="BH7" t="inlineStr"/>
       <c r="BI7" t="inlineStr"/>
+      <c r="BJ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1312,6 +1323,7 @@
       <c r="BG8" t="inlineStr"/>
       <c r="BH8" t="inlineStr"/>
       <c r="BI8" t="inlineStr"/>
+      <c r="BJ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1391,6 +1403,7 @@
       <c r="BG9" t="inlineStr"/>
       <c r="BH9" t="inlineStr"/>
       <c r="BI9" t="inlineStr"/>
+      <c r="BJ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1663,6 +1676,11 @@
       </c>
       <c r="BI10" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BJ10" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -1901,6 +1919,7 @@
         </is>
       </c>
       <c r="BI11" t="inlineStr"/>
+      <c r="BJ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2044,6 +2063,7 @@
         </is>
       </c>
       <c r="BI12" t="inlineStr"/>
+      <c r="BJ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2219,6 +2239,7 @@
       <c r="BG13" t="inlineStr"/>
       <c r="BH13" t="inlineStr"/>
       <c r="BI13" t="inlineStr"/>
+      <c r="BJ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2306,6 +2327,7 @@
       <c r="BG14" t="inlineStr"/>
       <c r="BH14" t="inlineStr"/>
       <c r="BI14" t="inlineStr"/>
+      <c r="BJ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2389,6 +2411,7 @@
       <c r="BG15" t="inlineStr"/>
       <c r="BH15" t="inlineStr"/>
       <c r="BI15" t="inlineStr"/>
+      <c r="BJ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2500,6 +2523,7 @@
       <c r="BG16" t="inlineStr"/>
       <c r="BH16" t="inlineStr"/>
       <c r="BI16" t="inlineStr"/>
+      <c r="BJ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2583,6 +2607,7 @@
       <c r="BG17" t="inlineStr"/>
       <c r="BH17" t="inlineStr"/>
       <c r="BI17" t="inlineStr"/>
+      <c r="BJ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2658,6 +2683,7 @@
       <c r="BG18" t="inlineStr"/>
       <c r="BH18" t="inlineStr"/>
       <c r="BI18" t="inlineStr"/>
+      <c r="BJ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2757,6 +2783,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BJ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2879,7 +2906,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BI20" t="inlineStr"/>
+      <c r="BI20" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BJ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2955,6 +2987,7 @@
       <c r="BG21" t="inlineStr"/>
       <c r="BH21" t="inlineStr"/>
       <c r="BI21" t="inlineStr"/>
+      <c r="BJ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3050,6 +3083,7 @@
         </is>
       </c>
       <c r="BI22" t="inlineStr"/>
+      <c r="BJ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3165,6 +3199,7 @@
       <c r="BG23" t="inlineStr"/>
       <c r="BH23" t="inlineStr"/>
       <c r="BI23" t="inlineStr"/>
+      <c r="BJ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3272,6 +3307,7 @@
       <c r="BG24" t="inlineStr"/>
       <c r="BH24" t="inlineStr"/>
       <c r="BI24" t="inlineStr"/>
+      <c r="BJ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3375,6 +3411,7 @@
       <c r="BG25" t="inlineStr"/>
       <c r="BH25" t="inlineStr"/>
       <c r="BI25" t="inlineStr"/>
+      <c r="BJ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3486,6 +3523,7 @@
       <c r="BG26" t="inlineStr"/>
       <c r="BH26" t="inlineStr"/>
       <c r="BI26" t="inlineStr"/>
+      <c r="BJ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3573,6 +3611,11 @@
       <c r="BG27" t="inlineStr"/>
       <c r="BH27" t="inlineStr"/>
       <c r="BI27" t="inlineStr"/>
+      <c r="BJ27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3648,6 +3691,7 @@
       <c r="BG28" t="inlineStr"/>
       <c r="BH28" t="inlineStr"/>
       <c r="BI28" t="inlineStr"/>
+      <c r="BJ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3735,6 +3779,7 @@
         </is>
       </c>
       <c r="BI29" t="inlineStr"/>
+      <c r="BJ29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3818,6 +3863,7 @@
         </is>
       </c>
       <c r="BI30" t="inlineStr"/>
+      <c r="BJ30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3893,6 +3939,7 @@
       <c r="BG31" t="inlineStr"/>
       <c r="BH31" t="inlineStr"/>
       <c r="BI31" t="inlineStr"/>
+      <c r="BJ31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3984,6 +4031,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BJ32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4059,6 +4107,7 @@
       <c r="BG33" t="inlineStr"/>
       <c r="BH33" t="inlineStr"/>
       <c r="BI33" t="inlineStr"/>
+      <c r="BJ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4134,6 +4183,7 @@
       <c r="BG34" t="inlineStr"/>
       <c r="BH34" t="inlineStr"/>
       <c r="BI34" t="inlineStr"/>
+      <c r="BJ34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4249,6 +4299,7 @@
         </is>
       </c>
       <c r="BI35" t="inlineStr"/>
+      <c r="BJ35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4352,6 +4403,7 @@
         </is>
       </c>
       <c r="BI36" t="inlineStr"/>
+      <c r="BJ36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4453,8 +4505,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BH37" t="inlineStr"/>
-      <c r="BI37" t="inlineStr"/>
+      <c r="BH37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BI37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BJ37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4530,6 +4591,7 @@
       <c r="BG38" t="inlineStr"/>
       <c r="BH38" t="inlineStr"/>
       <c r="BI38" t="inlineStr"/>
+      <c r="BJ38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4633,6 +4695,7 @@
       </c>
       <c r="BH39" t="inlineStr"/>
       <c r="BI39" t="inlineStr"/>
+      <c r="BJ39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4724,6 +4787,7 @@
         </is>
       </c>
       <c r="BI40" t="inlineStr"/>
+      <c r="BJ40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4807,6 +4871,7 @@
       <c r="BG41" t="inlineStr"/>
       <c r="BH41" t="inlineStr"/>
       <c r="BI41" t="inlineStr"/>
+      <c r="BJ41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4906,6 +4971,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BJ42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5005,6 +5071,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BJ43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5099,7 +5166,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BI44" t="inlineStr"/>
+      <c r="BI44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BJ44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5195,6 +5271,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BJ45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5270,6 +5347,7 @@
       <c r="BG46" t="inlineStr"/>
       <c r="BH46" t="inlineStr"/>
       <c r="BI46" t="inlineStr"/>
+      <c r="BJ46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5353,6 +5431,7 @@
       <c r="BG47" t="inlineStr"/>
       <c r="BH47" t="inlineStr"/>
       <c r="BI47" t="inlineStr"/>
+      <c r="BJ47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5428,6 +5507,7 @@
       </c>
       <c r="BH48" t="inlineStr"/>
       <c r="BI48" t="inlineStr"/>
+      <c r="BJ48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
## 분석 시간: 2025-05-30 09:47:21## 분석 시간: 2025-05-25 09:03:37
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ48"/>
+  <dimension ref="A1:BK48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,6 +742,11 @@
       <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
         </is>
       </c>
     </row>
@@ -816,6 +821,7 @@
       <c r="BH2" t="inlineStr"/>
       <c r="BI2" t="inlineStr"/>
       <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -912,6 +918,7 @@
       <c r="BH3" t="inlineStr"/>
       <c r="BI3" t="inlineStr"/>
       <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -996,6 +1003,7 @@
       <c r="BH4" t="inlineStr"/>
       <c r="BI4" t="inlineStr"/>
       <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1076,6 +1084,7 @@
       <c r="BH5" t="inlineStr"/>
       <c r="BI5" t="inlineStr"/>
       <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1159,7 +1168,12 @@
       <c r="BG6" t="inlineStr"/>
       <c r="BH6" t="inlineStr"/>
       <c r="BI6" t="inlineStr"/>
-      <c r="BJ6" t="inlineStr"/>
+      <c r="BJ6" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1240,6 +1254,7 @@
       <c r="BH7" t="inlineStr"/>
       <c r="BI7" t="inlineStr"/>
       <c r="BJ7" t="inlineStr"/>
+      <c r="BK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1324,6 +1339,7 @@
       <c r="BH8" t="inlineStr"/>
       <c r="BI8" t="inlineStr"/>
       <c r="BJ8" t="inlineStr"/>
+      <c r="BK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1404,6 +1420,7 @@
       <c r="BH9" t="inlineStr"/>
       <c r="BI9" t="inlineStr"/>
       <c r="BJ9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1681,6 +1698,11 @@
       </c>
       <c r="BJ10" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BK10" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -1920,6 +1942,7 @@
       </c>
       <c r="BI11" t="inlineStr"/>
       <c r="BJ11" t="inlineStr"/>
+      <c r="BK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2063,7 +2086,12 @@
         </is>
       </c>
       <c r="BI12" t="inlineStr"/>
-      <c r="BJ12" t="inlineStr"/>
+      <c r="BJ12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2240,6 +2268,7 @@
       <c r="BH13" t="inlineStr"/>
       <c r="BI13" t="inlineStr"/>
       <c r="BJ13" t="inlineStr"/>
+      <c r="BK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2328,6 +2357,7 @@
       <c r="BH14" t="inlineStr"/>
       <c r="BI14" t="inlineStr"/>
       <c r="BJ14" t="inlineStr"/>
+      <c r="BK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2412,6 +2442,7 @@
       <c r="BH15" t="inlineStr"/>
       <c r="BI15" t="inlineStr"/>
       <c r="BJ15" t="inlineStr"/>
+      <c r="BK15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2524,6 +2555,7 @@
       <c r="BH16" t="inlineStr"/>
       <c r="BI16" t="inlineStr"/>
       <c r="BJ16" t="inlineStr"/>
+      <c r="BK16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2608,6 +2640,7 @@
       <c r="BH17" t="inlineStr"/>
       <c r="BI17" t="inlineStr"/>
       <c r="BJ17" t="inlineStr"/>
+      <c r="BK17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2684,6 +2717,7 @@
       <c r="BH18" t="inlineStr"/>
       <c r="BI18" t="inlineStr"/>
       <c r="BJ18" t="inlineStr"/>
+      <c r="BK18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2784,6 +2818,7 @@
         </is>
       </c>
       <c r="BJ19" t="inlineStr"/>
+      <c r="BK19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2912,6 +2947,7 @@
         </is>
       </c>
       <c r="BJ20" t="inlineStr"/>
+      <c r="BK20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2988,6 +3024,7 @@
       <c r="BH21" t="inlineStr"/>
       <c r="BI21" t="inlineStr"/>
       <c r="BJ21" t="inlineStr"/>
+      <c r="BK21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3083,7 +3120,12 @@
         </is>
       </c>
       <c r="BI22" t="inlineStr"/>
-      <c r="BJ22" t="inlineStr"/>
+      <c r="BJ22" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3200,6 +3242,7 @@
       <c r="BH23" t="inlineStr"/>
       <c r="BI23" t="inlineStr"/>
       <c r="BJ23" t="inlineStr"/>
+      <c r="BK23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3308,6 +3351,7 @@
       <c r="BH24" t="inlineStr"/>
       <c r="BI24" t="inlineStr"/>
       <c r="BJ24" t="inlineStr"/>
+      <c r="BK24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3412,6 +3456,7 @@
       <c r="BH25" t="inlineStr"/>
       <c r="BI25" t="inlineStr"/>
       <c r="BJ25" t="inlineStr"/>
+      <c r="BK25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3524,6 +3569,7 @@
       <c r="BH26" t="inlineStr"/>
       <c r="BI26" t="inlineStr"/>
       <c r="BJ26" t="inlineStr"/>
+      <c r="BK26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3616,6 +3662,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BK27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3692,6 +3739,7 @@
       <c r="BH28" t="inlineStr"/>
       <c r="BI28" t="inlineStr"/>
       <c r="BJ28" t="inlineStr"/>
+      <c r="BK28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3779,7 +3827,12 @@
         </is>
       </c>
       <c r="BI29" t="inlineStr"/>
-      <c r="BJ29" t="inlineStr"/>
+      <c r="BJ29" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3864,6 +3917,7 @@
       </c>
       <c r="BI30" t="inlineStr"/>
       <c r="BJ30" t="inlineStr"/>
+      <c r="BK30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3939,7 +3993,12 @@
       <c r="BG31" t="inlineStr"/>
       <c r="BH31" t="inlineStr"/>
       <c r="BI31" t="inlineStr"/>
-      <c r="BJ31" t="inlineStr"/>
+      <c r="BJ31" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4031,7 +4090,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BJ32" t="inlineStr"/>
+      <c r="BJ32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4108,6 +4172,7 @@
       <c r="BH33" t="inlineStr"/>
       <c r="BI33" t="inlineStr"/>
       <c r="BJ33" t="inlineStr"/>
+      <c r="BK33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4184,6 +4249,7 @@
       <c r="BH34" t="inlineStr"/>
       <c r="BI34" t="inlineStr"/>
       <c r="BJ34" t="inlineStr"/>
+      <c r="BK34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4299,7 +4365,12 @@
         </is>
       </c>
       <c r="BI35" t="inlineStr"/>
-      <c r="BJ35" t="inlineStr"/>
+      <c r="BJ35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4404,6 +4475,7 @@
       </c>
       <c r="BI36" t="inlineStr"/>
       <c r="BJ36" t="inlineStr"/>
+      <c r="BK36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4515,7 +4587,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BJ37" t="inlineStr"/>
+      <c r="BJ37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4592,6 +4669,7 @@
       <c r="BH38" t="inlineStr"/>
       <c r="BI38" t="inlineStr"/>
       <c r="BJ38" t="inlineStr"/>
+      <c r="BK38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4696,6 +4774,7 @@
       <c r="BH39" t="inlineStr"/>
       <c r="BI39" t="inlineStr"/>
       <c r="BJ39" t="inlineStr"/>
+      <c r="BK39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4788,6 +4867,7 @@
       </c>
       <c r="BI40" t="inlineStr"/>
       <c r="BJ40" t="inlineStr"/>
+      <c r="BK40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4871,7 +4951,12 @@
       <c r="BG41" t="inlineStr"/>
       <c r="BH41" t="inlineStr"/>
       <c r="BI41" t="inlineStr"/>
-      <c r="BJ41" t="inlineStr"/>
+      <c r="BJ41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4971,7 +5056,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BJ42" t="inlineStr"/>
+      <c r="BJ42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5071,7 +5165,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BJ43" t="inlineStr"/>
+      <c r="BJ43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5176,6 +5275,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BK44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5271,7 +5371,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BJ45" t="inlineStr"/>
+      <c r="BJ45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5348,6 +5453,7 @@
       <c r="BH46" t="inlineStr"/>
       <c r="BI46" t="inlineStr"/>
       <c r="BJ46" t="inlineStr"/>
+      <c r="BK46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5432,6 +5538,7 @@
       <c r="BH47" t="inlineStr"/>
       <c r="BI47" t="inlineStr"/>
       <c r="BJ47" t="inlineStr"/>
+      <c r="BK47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5508,6 +5615,7 @@
       <c r="BH48" t="inlineStr"/>
       <c r="BI48" t="inlineStr"/>
       <c r="BJ48" t="inlineStr"/>
+      <c r="BK48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
## 분석 시간: 2025-05-31 08:35:43
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK48"/>
+  <dimension ref="A1:BL48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -747,6 +747,11 @@
       <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>2025-05-31</t>
         </is>
       </c>
     </row>
@@ -822,6 +827,7 @@
       <c r="BI2" t="inlineStr"/>
       <c r="BJ2" t="inlineStr"/>
       <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -919,6 +925,7 @@
       <c r="BI3" t="inlineStr"/>
       <c r="BJ3" t="inlineStr"/>
       <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1004,6 +1011,7 @@
       <c r="BI4" t="inlineStr"/>
       <c r="BJ4" t="inlineStr"/>
       <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1085,6 +1093,7 @@
       <c r="BI5" t="inlineStr"/>
       <c r="BJ5" t="inlineStr"/>
       <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1174,6 +1183,7 @@
         </is>
       </c>
       <c r="BK6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1255,6 +1265,7 @@
       <c r="BI7" t="inlineStr"/>
       <c r="BJ7" t="inlineStr"/>
       <c r="BK7" t="inlineStr"/>
+      <c r="BL7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1340,6 +1351,7 @@
       <c r="BI8" t="inlineStr"/>
       <c r="BJ8" t="inlineStr"/>
       <c r="BK8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1421,6 +1433,7 @@
       <c r="BI9" t="inlineStr"/>
       <c r="BJ9" t="inlineStr"/>
       <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1703,6 +1716,11 @@
       </c>
       <c r="BK10" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BL10" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -1943,6 +1961,7 @@
       <c r="BI11" t="inlineStr"/>
       <c r="BJ11" t="inlineStr"/>
       <c r="BK11" t="inlineStr"/>
+      <c r="BL11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2092,6 +2111,7 @@
         </is>
       </c>
       <c r="BK12" t="inlineStr"/>
+      <c r="BL12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2269,6 +2289,7 @@
       <c r="BI13" t="inlineStr"/>
       <c r="BJ13" t="inlineStr"/>
       <c r="BK13" t="inlineStr"/>
+      <c r="BL13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2358,6 +2379,7 @@
       <c r="BI14" t="inlineStr"/>
       <c r="BJ14" t="inlineStr"/>
       <c r="BK14" t="inlineStr"/>
+      <c r="BL14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2443,6 +2465,7 @@
       <c r="BI15" t="inlineStr"/>
       <c r="BJ15" t="inlineStr"/>
       <c r="BK15" t="inlineStr"/>
+      <c r="BL15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2556,6 +2579,7 @@
       <c r="BI16" t="inlineStr"/>
       <c r="BJ16" t="inlineStr"/>
       <c r="BK16" t="inlineStr"/>
+      <c r="BL16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2641,6 +2665,7 @@
       <c r="BI17" t="inlineStr"/>
       <c r="BJ17" t="inlineStr"/>
       <c r="BK17" t="inlineStr"/>
+      <c r="BL17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2718,6 +2743,7 @@
       <c r="BI18" t="inlineStr"/>
       <c r="BJ18" t="inlineStr"/>
       <c r="BK18" t="inlineStr"/>
+      <c r="BL18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2818,7 +2844,12 @@
         </is>
       </c>
       <c r="BJ19" t="inlineStr"/>
-      <c r="BK19" t="inlineStr"/>
+      <c r="BK19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2948,6 +2979,7 @@
       </c>
       <c r="BJ20" t="inlineStr"/>
       <c r="BK20" t="inlineStr"/>
+      <c r="BL20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3025,6 +3057,7 @@
       <c r="BI21" t="inlineStr"/>
       <c r="BJ21" t="inlineStr"/>
       <c r="BK21" t="inlineStr"/>
+      <c r="BL21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3126,6 +3159,7 @@
         </is>
       </c>
       <c r="BK22" t="inlineStr"/>
+      <c r="BL22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3243,6 +3277,7 @@
       <c r="BI23" t="inlineStr"/>
       <c r="BJ23" t="inlineStr"/>
       <c r="BK23" t="inlineStr"/>
+      <c r="BL23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3352,6 +3387,7 @@
       <c r="BI24" t="inlineStr"/>
       <c r="BJ24" t="inlineStr"/>
       <c r="BK24" t="inlineStr"/>
+      <c r="BL24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3457,6 +3493,7 @@
       <c r="BI25" t="inlineStr"/>
       <c r="BJ25" t="inlineStr"/>
       <c r="BK25" t="inlineStr"/>
+      <c r="BL25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3570,6 +3607,7 @@
       <c r="BI26" t="inlineStr"/>
       <c r="BJ26" t="inlineStr"/>
       <c r="BK26" t="inlineStr"/>
+      <c r="BL26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3663,6 +3701,7 @@
         </is>
       </c>
       <c r="BK27" t="inlineStr"/>
+      <c r="BL27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3740,6 +3779,7 @@
       <c r="BI28" t="inlineStr"/>
       <c r="BJ28" t="inlineStr"/>
       <c r="BK28" t="inlineStr"/>
+      <c r="BL28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3833,6 +3873,7 @@
         </is>
       </c>
       <c r="BK29" t="inlineStr"/>
+      <c r="BL29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3917,7 +3958,12 @@
       </c>
       <c r="BI30" t="inlineStr"/>
       <c r="BJ30" t="inlineStr"/>
-      <c r="BK30" t="inlineStr"/>
+      <c r="BK30" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3998,7 +4044,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK31" t="inlineStr"/>
+      <c r="BK31" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4095,7 +4146,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK32" t="inlineStr"/>
+      <c r="BK32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4173,6 +4229,7 @@
       <c r="BI33" t="inlineStr"/>
       <c r="BJ33" t="inlineStr"/>
       <c r="BK33" t="inlineStr"/>
+      <c r="BL33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4250,6 +4307,7 @@
       <c r="BI34" t="inlineStr"/>
       <c r="BJ34" t="inlineStr"/>
       <c r="BK34" t="inlineStr"/>
+      <c r="BL34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4370,7 +4428,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK35" t="inlineStr"/>
+      <c r="BK35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4476,6 +4539,7 @@
       <c r="BI36" t="inlineStr"/>
       <c r="BJ36" t="inlineStr"/>
       <c r="BK36" t="inlineStr"/>
+      <c r="BL36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4593,6 +4657,7 @@
         </is>
       </c>
       <c r="BK37" t="inlineStr"/>
+      <c r="BL37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4670,6 +4735,7 @@
       <c r="BI38" t="inlineStr"/>
       <c r="BJ38" t="inlineStr"/>
       <c r="BK38" t="inlineStr"/>
+      <c r="BL38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4775,6 +4841,7 @@
       <c r="BI39" t="inlineStr"/>
       <c r="BJ39" t="inlineStr"/>
       <c r="BK39" t="inlineStr"/>
+      <c r="BL39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4868,6 +4935,7 @@
       <c r="BI40" t="inlineStr"/>
       <c r="BJ40" t="inlineStr"/>
       <c r="BK40" t="inlineStr"/>
+      <c r="BL40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4957,6 +5025,7 @@
         </is>
       </c>
       <c r="BK41" t="inlineStr"/>
+      <c r="BL41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5066,6 +5135,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BL42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5170,7 +5240,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK43" t="inlineStr"/>
+      <c r="BK43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5276,6 +5351,7 @@
         </is>
       </c>
       <c r="BK44" t="inlineStr"/>
+      <c r="BL44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5376,7 +5452,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK45" t="inlineStr"/>
+      <c r="BK45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5454,6 +5535,7 @@
       <c r="BI46" t="inlineStr"/>
       <c r="BJ46" t="inlineStr"/>
       <c r="BK46" t="inlineStr"/>
+      <c r="BL46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5539,6 +5621,7 @@
       <c r="BI47" t="inlineStr"/>
       <c r="BJ47" t="inlineStr"/>
       <c r="BK47" t="inlineStr"/>
+      <c r="BL47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5616,6 +5699,7 @@
       <c r="BI48" t="inlineStr"/>
       <c r="BJ48" t="inlineStr"/>
       <c r="BK48" t="inlineStr"/>
+      <c r="BL48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-01 12:14:51
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL48"/>
+  <dimension ref="A1:BM48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,6 +752,11 @@
       <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
         </is>
       </c>
     </row>
@@ -828,6 +833,7 @@
       <c r="BJ2" t="inlineStr"/>
       <c r="BK2" t="inlineStr"/>
       <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -926,6 +932,7 @@
       <c r="BJ3" t="inlineStr"/>
       <c r="BK3" t="inlineStr"/>
       <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1012,6 +1019,7 @@
       <c r="BJ4" t="inlineStr"/>
       <c r="BK4" t="inlineStr"/>
       <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1094,6 +1102,7 @@
       <c r="BJ5" t="inlineStr"/>
       <c r="BK5" t="inlineStr"/>
       <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1184,6 +1193,7 @@
       </c>
       <c r="BK6" t="inlineStr"/>
       <c r="BL6" t="inlineStr"/>
+      <c r="BM6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1266,6 +1276,7 @@
       <c r="BJ7" t="inlineStr"/>
       <c r="BK7" t="inlineStr"/>
       <c r="BL7" t="inlineStr"/>
+      <c r="BM7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1352,6 +1363,7 @@
       <c r="BJ8" t="inlineStr"/>
       <c r="BK8" t="inlineStr"/>
       <c r="BL8" t="inlineStr"/>
+      <c r="BM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1434,6 +1446,7 @@
       <c r="BJ9" t="inlineStr"/>
       <c r="BK9" t="inlineStr"/>
       <c r="BL9" t="inlineStr"/>
+      <c r="BM9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1721,9 +1734,10 @@
       </c>
       <c r="BL10" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BM10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1961,7 +1975,16 @@
       <c r="BI11" t="inlineStr"/>
       <c r="BJ11" t="inlineStr"/>
       <c r="BK11" t="inlineStr"/>
-      <c r="BL11" t="inlineStr"/>
+      <c r="BL11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2111,7 +2134,12 @@
         </is>
       </c>
       <c r="BK12" t="inlineStr"/>
-      <c r="BL12" t="inlineStr"/>
+      <c r="BL12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2289,7 +2317,12 @@
       <c r="BI13" t="inlineStr"/>
       <c r="BJ13" t="inlineStr"/>
       <c r="BK13" t="inlineStr"/>
-      <c r="BL13" t="inlineStr"/>
+      <c r="BL13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2380,6 +2413,7 @@
       <c r="BJ14" t="inlineStr"/>
       <c r="BK14" t="inlineStr"/>
       <c r="BL14" t="inlineStr"/>
+      <c r="BM14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2466,6 +2500,7 @@
       <c r="BJ15" t="inlineStr"/>
       <c r="BK15" t="inlineStr"/>
       <c r="BL15" t="inlineStr"/>
+      <c r="BM15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2580,6 +2615,7 @@
       <c r="BJ16" t="inlineStr"/>
       <c r="BK16" t="inlineStr"/>
       <c r="BL16" t="inlineStr"/>
+      <c r="BM16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2666,6 +2702,7 @@
       <c r="BJ17" t="inlineStr"/>
       <c r="BK17" t="inlineStr"/>
       <c r="BL17" t="inlineStr"/>
+      <c r="BM17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2744,6 +2781,7 @@
       <c r="BJ18" t="inlineStr"/>
       <c r="BK18" t="inlineStr"/>
       <c r="BL18" t="inlineStr"/>
+      <c r="BM18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2850,6 +2888,7 @@
         </is>
       </c>
       <c r="BL19" t="inlineStr"/>
+      <c r="BM19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2980,6 +3019,7 @@
       <c r="BJ20" t="inlineStr"/>
       <c r="BK20" t="inlineStr"/>
       <c r="BL20" t="inlineStr"/>
+      <c r="BM20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3058,6 +3098,7 @@
       <c r="BJ21" t="inlineStr"/>
       <c r="BK21" t="inlineStr"/>
       <c r="BL21" t="inlineStr"/>
+      <c r="BM21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3160,6 +3201,11 @@
       </c>
       <c r="BK22" t="inlineStr"/>
       <c r="BL22" t="inlineStr"/>
+      <c r="BM22" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3278,6 +3324,7 @@
       <c r="BJ23" t="inlineStr"/>
       <c r="BK23" t="inlineStr"/>
       <c r="BL23" t="inlineStr"/>
+      <c r="BM23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3388,6 +3435,7 @@
       <c r="BJ24" t="inlineStr"/>
       <c r="BK24" t="inlineStr"/>
       <c r="BL24" t="inlineStr"/>
+      <c r="BM24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3494,6 +3542,7 @@
       <c r="BJ25" t="inlineStr"/>
       <c r="BK25" t="inlineStr"/>
       <c r="BL25" t="inlineStr"/>
+      <c r="BM25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3608,6 +3657,7 @@
       <c r="BJ26" t="inlineStr"/>
       <c r="BK26" t="inlineStr"/>
       <c r="BL26" t="inlineStr"/>
+      <c r="BM26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3702,6 +3752,7 @@
       </c>
       <c r="BK27" t="inlineStr"/>
       <c r="BL27" t="inlineStr"/>
+      <c r="BM27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3780,6 +3831,7 @@
       <c r="BJ28" t="inlineStr"/>
       <c r="BK28" t="inlineStr"/>
       <c r="BL28" t="inlineStr"/>
+      <c r="BM28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3874,6 +3926,7 @@
       </c>
       <c r="BK29" t="inlineStr"/>
       <c r="BL29" t="inlineStr"/>
+      <c r="BM29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3964,6 +4017,7 @@
         </is>
       </c>
       <c r="BL30" t="inlineStr"/>
+      <c r="BM30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4049,7 +4103,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BL31" t="inlineStr"/>
+      <c r="BL31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BM31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4151,7 +4210,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BL32" t="inlineStr"/>
+      <c r="BL32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4230,6 +4294,7 @@
       <c r="BJ33" t="inlineStr"/>
       <c r="BK33" t="inlineStr"/>
       <c r="BL33" t="inlineStr"/>
+      <c r="BM33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4308,6 +4373,7 @@
       <c r="BJ34" t="inlineStr"/>
       <c r="BK34" t="inlineStr"/>
       <c r="BL34" t="inlineStr"/>
+      <c r="BM34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4433,7 +4499,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BL35" t="inlineStr"/>
+      <c r="BL35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4539,7 +4610,16 @@
       <c r="BI36" t="inlineStr"/>
       <c r="BJ36" t="inlineStr"/>
       <c r="BK36" t="inlineStr"/>
-      <c r="BL36" t="inlineStr"/>
+      <c r="BL36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4656,8 +4736,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BK37" t="inlineStr"/>
-      <c r="BL37" t="inlineStr"/>
+      <c r="BK37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL37" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BM37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4736,6 +4825,7 @@
       <c r="BJ38" t="inlineStr"/>
       <c r="BK38" t="inlineStr"/>
       <c r="BL38" t="inlineStr"/>
+      <c r="BM38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4842,6 +4932,7 @@
       <c r="BJ39" t="inlineStr"/>
       <c r="BK39" t="inlineStr"/>
       <c r="BL39" t="inlineStr"/>
+      <c r="BM39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4936,6 +5027,7 @@
       <c r="BJ40" t="inlineStr"/>
       <c r="BK40" t="inlineStr"/>
       <c r="BL40" t="inlineStr"/>
+      <c r="BM40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5025,7 +5117,16 @@
         </is>
       </c>
       <c r="BK41" t="inlineStr"/>
-      <c r="BL41" t="inlineStr"/>
+      <c r="BL41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5135,7 +5236,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BL42" t="inlineStr"/>
+      <c r="BL42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BM42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5245,7 +5351,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BL43" t="inlineStr"/>
+      <c r="BL43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5352,6 +5467,11 @@
       </c>
       <c r="BK44" t="inlineStr"/>
       <c r="BL44" t="inlineStr"/>
+      <c r="BM44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5458,6 +5578,7 @@
         </is>
       </c>
       <c r="BL45" t="inlineStr"/>
+      <c r="BM45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5536,6 +5657,7 @@
       <c r="BJ46" t="inlineStr"/>
       <c r="BK46" t="inlineStr"/>
       <c r="BL46" t="inlineStr"/>
+      <c r="BM46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5622,6 +5744,7 @@
       <c r="BJ47" t="inlineStr"/>
       <c r="BK47" t="inlineStr"/>
       <c r="BL47" t="inlineStr"/>
+      <c r="BM47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5700,6 +5823,7 @@
       <c r="BJ48" t="inlineStr"/>
       <c r="BK48" t="inlineStr"/>
       <c r="BL48" t="inlineStr"/>
+      <c r="BM48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
## 분석 시간: 2025-06-02 02:48:59
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM48"/>
+  <dimension ref="A1:BN48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,6 +757,11 @@
       <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>2025-06-01</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
         </is>
       </c>
     </row>
@@ -834,6 +839,7 @@
       <c r="BK2" t="inlineStr"/>
       <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -933,6 +939,7 @@
       <c r="BK3" t="inlineStr"/>
       <c r="BL3" t="inlineStr"/>
       <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1020,6 +1027,7 @@
       <c r="BK4" t="inlineStr"/>
       <c r="BL4" t="inlineStr"/>
       <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1103,6 +1111,7 @@
       <c r="BK5" t="inlineStr"/>
       <c r="BL5" t="inlineStr"/>
       <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1194,6 +1203,7 @@
       <c r="BK6" t="inlineStr"/>
       <c r="BL6" t="inlineStr"/>
       <c r="BM6" t="inlineStr"/>
+      <c r="BN6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1277,6 +1287,7 @@
       <c r="BK7" t="inlineStr"/>
       <c r="BL7" t="inlineStr"/>
       <c r="BM7" t="inlineStr"/>
+      <c r="BN7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1364,6 +1375,7 @@
       <c r="BK8" t="inlineStr"/>
       <c r="BL8" t="inlineStr"/>
       <c r="BM8" t="inlineStr"/>
+      <c r="BN8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1447,6 +1459,7 @@
       <c r="BK9" t="inlineStr"/>
       <c r="BL9" t="inlineStr"/>
       <c r="BM9" t="inlineStr"/>
+      <c r="BN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1737,7 +1750,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BM10" t="inlineStr"/>
+      <c r="BM10" t="inlineStr">
+        <is>
+          <t>대화 (80.4kg)</t>
+        </is>
+      </c>
+      <c r="BN10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1985,6 +2003,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2139,7 +2158,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BM12" t="inlineStr"/>
+      <c r="BM12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BN12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2323,6 +2347,7 @@
         </is>
       </c>
       <c r="BM13" t="inlineStr"/>
+      <c r="BN13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2414,6 +2439,7 @@
       <c r="BK14" t="inlineStr"/>
       <c r="BL14" t="inlineStr"/>
       <c r="BM14" t="inlineStr"/>
+      <c r="BN14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2501,6 +2527,7 @@
       <c r="BK15" t="inlineStr"/>
       <c r="BL15" t="inlineStr"/>
       <c r="BM15" t="inlineStr"/>
+      <c r="BN15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2616,6 +2643,7 @@
       <c r="BK16" t="inlineStr"/>
       <c r="BL16" t="inlineStr"/>
       <c r="BM16" t="inlineStr"/>
+      <c r="BN16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2703,6 +2731,7 @@
       <c r="BK17" t="inlineStr"/>
       <c r="BL17" t="inlineStr"/>
       <c r="BM17" t="inlineStr"/>
+      <c r="BN17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2782,6 +2811,7 @@
       <c r="BK18" t="inlineStr"/>
       <c r="BL18" t="inlineStr"/>
       <c r="BM18" t="inlineStr"/>
+      <c r="BN18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2889,6 +2919,7 @@
       </c>
       <c r="BL19" t="inlineStr"/>
       <c r="BM19" t="inlineStr"/>
+      <c r="BN19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3020,6 +3051,7 @@
       <c r="BK20" t="inlineStr"/>
       <c r="BL20" t="inlineStr"/>
       <c r="BM20" t="inlineStr"/>
+      <c r="BN20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3099,6 +3131,7 @@
       <c r="BK21" t="inlineStr"/>
       <c r="BL21" t="inlineStr"/>
       <c r="BM21" t="inlineStr"/>
+      <c r="BN21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3206,6 +3239,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3325,6 +3359,7 @@
       <c r="BK23" t="inlineStr"/>
       <c r="BL23" t="inlineStr"/>
       <c r="BM23" t="inlineStr"/>
+      <c r="BN23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3436,6 +3471,7 @@
       <c r="BK24" t="inlineStr"/>
       <c r="BL24" t="inlineStr"/>
       <c r="BM24" t="inlineStr"/>
+      <c r="BN24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3543,6 +3579,7 @@
       <c r="BK25" t="inlineStr"/>
       <c r="BL25" t="inlineStr"/>
       <c r="BM25" t="inlineStr"/>
+      <c r="BN25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3658,6 +3695,7 @@
       <c r="BK26" t="inlineStr"/>
       <c r="BL26" t="inlineStr"/>
       <c r="BM26" t="inlineStr"/>
+      <c r="BN26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3753,6 +3791,7 @@
       <c r="BK27" t="inlineStr"/>
       <c r="BL27" t="inlineStr"/>
       <c r="BM27" t="inlineStr"/>
+      <c r="BN27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3832,6 +3871,7 @@
       <c r="BK28" t="inlineStr"/>
       <c r="BL28" t="inlineStr"/>
       <c r="BM28" t="inlineStr"/>
+      <c r="BN28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3927,6 +3967,7 @@
       <c r="BK29" t="inlineStr"/>
       <c r="BL29" t="inlineStr"/>
       <c r="BM29" t="inlineStr"/>
+      <c r="BN29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4017,7 +4058,12 @@
         </is>
       </c>
       <c r="BL30" t="inlineStr"/>
-      <c r="BM30" t="inlineStr"/>
+      <c r="BM30" t="inlineStr">
+        <is>
+          <t>대화 (122.0kg)</t>
+        </is>
+      </c>
+      <c r="BN30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4108,7 +4154,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BM31" t="inlineStr"/>
+      <c r="BM31" t="inlineStr">
+        <is>
+          <t>대화 (72.5kg)</t>
+        </is>
+      </c>
+      <c r="BN31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4216,6 +4267,7 @@
         </is>
       </c>
       <c r="BM32" t="inlineStr"/>
+      <c r="BN32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4295,6 +4347,7 @@
       <c r="BK33" t="inlineStr"/>
       <c r="BL33" t="inlineStr"/>
       <c r="BM33" t="inlineStr"/>
+      <c r="BN33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4374,6 +4427,7 @@
       <c r="BK34" t="inlineStr"/>
       <c r="BL34" t="inlineStr"/>
       <c r="BM34" t="inlineStr"/>
+      <c r="BN34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4504,7 +4558,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BM35" t="inlineStr"/>
+      <c r="BM35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BN35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4620,6 +4679,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4747,6 +4807,7 @@
         </is>
       </c>
       <c r="BM37" t="inlineStr"/>
+      <c r="BN37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4826,6 +4887,7 @@
       <c r="BK38" t="inlineStr"/>
       <c r="BL38" t="inlineStr"/>
       <c r="BM38" t="inlineStr"/>
+      <c r="BN38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4933,6 +4995,7 @@
       <c r="BK39" t="inlineStr"/>
       <c r="BL39" t="inlineStr"/>
       <c r="BM39" t="inlineStr"/>
+      <c r="BN39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5028,6 +5091,7 @@
       <c r="BK40" t="inlineStr"/>
       <c r="BL40" t="inlineStr"/>
       <c r="BM40" t="inlineStr"/>
+      <c r="BN40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5127,6 +5191,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5241,7 +5306,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BM42" t="inlineStr"/>
+      <c r="BM42" t="inlineStr">
+        <is>
+          <t>대화 (97.3kg)</t>
+        </is>
+      </c>
+      <c r="BN42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5361,6 +5431,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5472,6 +5543,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BN44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5579,6 +5651,7 @@
       </c>
       <c r="BL45" t="inlineStr"/>
       <c r="BM45" t="inlineStr"/>
+      <c r="BN45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5658,6 +5731,7 @@
       <c r="BK46" t="inlineStr"/>
       <c r="BL46" t="inlineStr"/>
       <c r="BM46" t="inlineStr"/>
+      <c r="BN46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5745,6 +5819,7 @@
       <c r="BK47" t="inlineStr"/>
       <c r="BL47" t="inlineStr"/>
       <c r="BM47" t="inlineStr"/>
+      <c r="BN47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5824,6 +5899,7 @@
       <c r="BK48" t="inlineStr"/>
       <c r="BL48" t="inlineStr"/>
       <c r="BM48" t="inlineStr"/>
+      <c r="BN48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-03 13:01:54
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BN48"/>
+  <dimension ref="A1:BO48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,6 +762,11 @@
       <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
         </is>
       </c>
     </row>
@@ -840,6 +845,7 @@
       <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr"/>
       <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -940,6 +946,7 @@
       <c r="BL3" t="inlineStr"/>
       <c r="BM3" t="inlineStr"/>
       <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1028,6 +1035,7 @@
       <c r="BL4" t="inlineStr"/>
       <c r="BM4" t="inlineStr"/>
       <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1112,6 +1120,7 @@
       <c r="BL5" t="inlineStr"/>
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1204,6 +1213,7 @@
       <c r="BL6" t="inlineStr"/>
       <c r="BM6" t="inlineStr"/>
       <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1288,6 +1298,7 @@
       <c r="BL7" t="inlineStr"/>
       <c r="BM7" t="inlineStr"/>
       <c r="BN7" t="inlineStr"/>
+      <c r="BO7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1376,6 +1387,7 @@
       <c r="BL8" t="inlineStr"/>
       <c r="BM8" t="inlineStr"/>
       <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1460,6 +1472,7 @@
       <c r="BL9" t="inlineStr"/>
       <c r="BM9" t="inlineStr"/>
       <c r="BN9" t="inlineStr"/>
+      <c r="BO9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1755,7 +1768,12 @@
           <t>대화 (80.4kg)</t>
         </is>
       </c>
-      <c r="BN10" t="inlineStr"/>
+      <c r="BN10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BO10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2003,7 +2021,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BN11" t="inlineStr"/>
+      <c r="BN11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2164,6 +2187,7 @@
         </is>
       </c>
       <c r="BN12" t="inlineStr"/>
+      <c r="BO12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2348,6 +2372,7 @@
       </c>
       <c r="BM13" t="inlineStr"/>
       <c r="BN13" t="inlineStr"/>
+      <c r="BO13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2440,6 +2465,7 @@
       <c r="BL14" t="inlineStr"/>
       <c r="BM14" t="inlineStr"/>
       <c r="BN14" t="inlineStr"/>
+      <c r="BO14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2528,6 +2554,7 @@
       <c r="BL15" t="inlineStr"/>
       <c r="BM15" t="inlineStr"/>
       <c r="BN15" t="inlineStr"/>
+      <c r="BO15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2644,6 +2671,7 @@
       <c r="BL16" t="inlineStr"/>
       <c r="BM16" t="inlineStr"/>
       <c r="BN16" t="inlineStr"/>
+      <c r="BO16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2732,6 +2760,7 @@
       <c r="BL17" t="inlineStr"/>
       <c r="BM17" t="inlineStr"/>
       <c r="BN17" t="inlineStr"/>
+      <c r="BO17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2812,6 +2841,7 @@
       <c r="BL18" t="inlineStr"/>
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr"/>
+      <c r="BO18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2920,6 +2950,7 @@
       <c r="BL19" t="inlineStr"/>
       <c r="BM19" t="inlineStr"/>
       <c r="BN19" t="inlineStr"/>
+      <c r="BO19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3052,6 +3083,7 @@
       <c r="BL20" t="inlineStr"/>
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr"/>
+      <c r="BO20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3132,6 +3164,7 @@
       <c r="BL21" t="inlineStr"/>
       <c r="BM21" t="inlineStr"/>
       <c r="BN21" t="inlineStr"/>
+      <c r="BO21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3240,6 +3273,7 @@
         </is>
       </c>
       <c r="BN22" t="inlineStr"/>
+      <c r="BO22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3360,6 +3394,7 @@
       <c r="BL23" t="inlineStr"/>
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr"/>
+      <c r="BO23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3471,7 +3506,12 @@
       <c r="BK24" t="inlineStr"/>
       <c r="BL24" t="inlineStr"/>
       <c r="BM24" t="inlineStr"/>
-      <c r="BN24" t="inlineStr"/>
+      <c r="BN24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3580,6 +3620,7 @@
       <c r="BL25" t="inlineStr"/>
       <c r="BM25" t="inlineStr"/>
       <c r="BN25" t="inlineStr"/>
+      <c r="BO25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3696,6 +3737,11 @@
       <c r="BL26" t="inlineStr"/>
       <c r="BM26" t="inlineStr"/>
       <c r="BN26" t="inlineStr"/>
+      <c r="BO26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3792,6 +3838,7 @@
       <c r="BL27" t="inlineStr"/>
       <c r="BM27" t="inlineStr"/>
       <c r="BN27" t="inlineStr"/>
+      <c r="BO27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3872,6 +3919,7 @@
       <c r="BL28" t="inlineStr"/>
       <c r="BM28" t="inlineStr"/>
       <c r="BN28" t="inlineStr"/>
+      <c r="BO28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3967,7 +4015,16 @@
       <c r="BK29" t="inlineStr"/>
       <c r="BL29" t="inlineStr"/>
       <c r="BM29" t="inlineStr"/>
-      <c r="BN29" t="inlineStr"/>
+      <c r="BN29" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO29" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4064,6 +4121,7 @@
         </is>
       </c>
       <c r="BN30" t="inlineStr"/>
+      <c r="BO30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4159,7 +4217,12 @@
           <t>대화 (72.5kg)</t>
         </is>
       </c>
-      <c r="BN31" t="inlineStr"/>
+      <c r="BN31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BO31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4266,8 +4329,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BM32" t="inlineStr"/>
-      <c r="BN32" t="inlineStr"/>
+      <c r="BM32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BN32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4348,6 +4420,7 @@
       <c r="BL33" t="inlineStr"/>
       <c r="BM33" t="inlineStr"/>
       <c r="BN33" t="inlineStr"/>
+      <c r="BO33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4428,6 +4501,7 @@
       <c r="BL34" t="inlineStr"/>
       <c r="BM34" t="inlineStr"/>
       <c r="BN34" t="inlineStr"/>
+      <c r="BO34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4564,6 +4638,7 @@
         </is>
       </c>
       <c r="BN35" t="inlineStr"/>
+      <c r="BO35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4680,6 +4755,7 @@
         </is>
       </c>
       <c r="BN36" t="inlineStr"/>
+      <c r="BO36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4808,6 +4884,7 @@
       </c>
       <c r="BM37" t="inlineStr"/>
       <c r="BN37" t="inlineStr"/>
+      <c r="BO37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4888,6 +4965,7 @@
       <c r="BL38" t="inlineStr"/>
       <c r="BM38" t="inlineStr"/>
       <c r="BN38" t="inlineStr"/>
+      <c r="BO38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4996,6 +5074,7 @@
       <c r="BL39" t="inlineStr"/>
       <c r="BM39" t="inlineStr"/>
       <c r="BN39" t="inlineStr"/>
+      <c r="BO39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5092,6 +5171,7 @@
       <c r="BL40" t="inlineStr"/>
       <c r="BM40" t="inlineStr"/>
       <c r="BN40" t="inlineStr"/>
+      <c r="BO40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5192,6 +5272,7 @@
         </is>
       </c>
       <c r="BN41" t="inlineStr"/>
+      <c r="BO41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5311,7 +5392,16 @@
           <t>대화 (97.3kg)</t>
         </is>
       </c>
-      <c r="BN42" t="inlineStr"/>
+      <c r="BN42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BO42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5431,7 +5521,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BN43" t="inlineStr"/>
+      <c r="BN43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5543,7 +5642,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BN44" t="inlineStr"/>
+      <c r="BN44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5651,7 +5759,12 @@
       </c>
       <c r="BL45" t="inlineStr"/>
       <c r="BM45" t="inlineStr"/>
-      <c r="BN45" t="inlineStr"/>
+      <c r="BN45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5732,6 +5845,7 @@
       <c r="BL46" t="inlineStr"/>
       <c r="BM46" t="inlineStr"/>
       <c r="BN46" t="inlineStr"/>
+      <c r="BO46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5820,6 +5934,7 @@
       <c r="BL47" t="inlineStr"/>
       <c r="BM47" t="inlineStr"/>
       <c r="BN47" t="inlineStr"/>
+      <c r="BO47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5900,6 +6015,7 @@
       <c r="BL48" t="inlineStr"/>
       <c r="BM48" t="inlineStr"/>
       <c r="BN48" t="inlineStr"/>
+      <c r="BO48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-04 11:47:05
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BO48"/>
+  <dimension ref="A1:BP48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +767,11 @@
       <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>2025-06-03</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
         </is>
       </c>
     </row>
@@ -846,6 +851,7 @@
       <c r="BM2" t="inlineStr"/>
       <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -947,6 +953,7 @@
       <c r="BM3" t="inlineStr"/>
       <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1036,6 +1043,7 @@
       <c r="BM4" t="inlineStr"/>
       <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1121,6 +1129,7 @@
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr"/>
+      <c r="BP5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1214,6 +1223,7 @@
       <c r="BM6" t="inlineStr"/>
       <c r="BN6" t="inlineStr"/>
       <c r="BO6" t="inlineStr"/>
+      <c r="BP6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1299,6 +1309,7 @@
       <c r="BM7" t="inlineStr"/>
       <c r="BN7" t="inlineStr"/>
       <c r="BO7" t="inlineStr"/>
+      <c r="BP7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1388,6 +1399,7 @@
       <c r="BM8" t="inlineStr"/>
       <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="inlineStr"/>
+      <c r="BP8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1473,6 +1485,7 @@
       <c r="BM9" t="inlineStr"/>
       <c r="BN9" t="inlineStr"/>
       <c r="BO9" t="inlineStr"/>
+      <c r="BP9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1773,7 +1786,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BO10" t="inlineStr"/>
+      <c r="BO10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BP10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2027,6 +2045,7 @@
         </is>
       </c>
       <c r="BO11" t="inlineStr"/>
+      <c r="BP11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2188,6 +2207,7 @@
       </c>
       <c r="BN12" t="inlineStr"/>
       <c r="BO12" t="inlineStr"/>
+      <c r="BP12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2373,6 +2393,7 @@
       <c r="BM13" t="inlineStr"/>
       <c r="BN13" t="inlineStr"/>
       <c r="BO13" t="inlineStr"/>
+      <c r="BP13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2466,6 +2487,7 @@
       <c r="BM14" t="inlineStr"/>
       <c r="BN14" t="inlineStr"/>
       <c r="BO14" t="inlineStr"/>
+      <c r="BP14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2555,6 +2577,7 @@
       <c r="BM15" t="inlineStr"/>
       <c r="BN15" t="inlineStr"/>
       <c r="BO15" t="inlineStr"/>
+      <c r="BP15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2672,6 +2695,7 @@
       <c r="BM16" t="inlineStr"/>
       <c r="BN16" t="inlineStr"/>
       <c r="BO16" t="inlineStr"/>
+      <c r="BP16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2761,6 +2785,7 @@
       <c r="BM17" t="inlineStr"/>
       <c r="BN17" t="inlineStr"/>
       <c r="BO17" t="inlineStr"/>
+      <c r="BP17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2842,6 +2867,7 @@
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr"/>
       <c r="BO18" t="inlineStr"/>
+      <c r="BP18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2951,6 +2977,7 @@
       <c r="BM19" t="inlineStr"/>
       <c r="BN19" t="inlineStr"/>
       <c r="BO19" t="inlineStr"/>
+      <c r="BP19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3084,6 +3111,7 @@
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr"/>
       <c r="BO20" t="inlineStr"/>
+      <c r="BP20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3165,6 +3193,7 @@
       <c r="BM21" t="inlineStr"/>
       <c r="BN21" t="inlineStr"/>
       <c r="BO21" t="inlineStr"/>
+      <c r="BP21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3274,6 +3303,7 @@
       </c>
       <c r="BN22" t="inlineStr"/>
       <c r="BO22" t="inlineStr"/>
+      <c r="BP22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3395,6 +3425,7 @@
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr"/>
       <c r="BO23" t="inlineStr"/>
+      <c r="BP23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3512,6 +3543,7 @@
         </is>
       </c>
       <c r="BO24" t="inlineStr"/>
+      <c r="BP24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3621,6 +3653,11 @@
       <c r="BM25" t="inlineStr"/>
       <c r="BN25" t="inlineStr"/>
       <c r="BO25" t="inlineStr"/>
+      <c r="BP25" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3742,6 +3779,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BP26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3839,6 +3877,7 @@
       <c r="BM27" t="inlineStr"/>
       <c r="BN27" t="inlineStr"/>
       <c r="BO27" t="inlineStr"/>
+      <c r="BP27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3920,6 +3959,7 @@
       <c r="BM28" t="inlineStr"/>
       <c r="BN28" t="inlineStr"/>
       <c r="BO28" t="inlineStr"/>
+      <c r="BP28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4025,6 +4065,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BP29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4122,6 +4163,7 @@
       </c>
       <c r="BN30" t="inlineStr"/>
       <c r="BO30" t="inlineStr"/>
+      <c r="BP30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4222,7 +4264,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BO31" t="inlineStr"/>
+      <c r="BO31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BP31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4340,6 +4387,7 @@
         </is>
       </c>
       <c r="BO32" t="inlineStr"/>
+      <c r="BP32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4421,6 +4469,7 @@
       <c r="BM33" t="inlineStr"/>
       <c r="BN33" t="inlineStr"/>
       <c r="BO33" t="inlineStr"/>
+      <c r="BP33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4502,6 +4551,7 @@
       <c r="BM34" t="inlineStr"/>
       <c r="BN34" t="inlineStr"/>
       <c r="BO34" t="inlineStr"/>
+      <c r="BP34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4638,7 +4688,12 @@
         </is>
       </c>
       <c r="BN35" t="inlineStr"/>
-      <c r="BO35" t="inlineStr"/>
+      <c r="BO35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BP35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4756,6 +4811,7 @@
       </c>
       <c r="BN36" t="inlineStr"/>
       <c r="BO36" t="inlineStr"/>
+      <c r="BP36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4885,6 +4941,7 @@
       <c r="BM37" t="inlineStr"/>
       <c r="BN37" t="inlineStr"/>
       <c r="BO37" t="inlineStr"/>
+      <c r="BP37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4966,6 +5023,7 @@
       <c r="BM38" t="inlineStr"/>
       <c r="BN38" t="inlineStr"/>
       <c r="BO38" t="inlineStr"/>
+      <c r="BP38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5075,6 +5133,7 @@
       <c r="BM39" t="inlineStr"/>
       <c r="BN39" t="inlineStr"/>
       <c r="BO39" t="inlineStr"/>
+      <c r="BP39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5172,6 +5231,7 @@
       <c r="BM40" t="inlineStr"/>
       <c r="BN40" t="inlineStr"/>
       <c r="BO40" t="inlineStr"/>
+      <c r="BP40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5273,6 +5333,7 @@
       </c>
       <c r="BN41" t="inlineStr"/>
       <c r="BO41" t="inlineStr"/>
+      <c r="BP41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5399,9 +5460,10 @@
       </c>
       <c r="BO42" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BP42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5531,6 +5593,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BP43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5652,6 +5715,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BP44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5765,6 +5829,7 @@
         </is>
       </c>
       <c r="BO45" t="inlineStr"/>
+      <c r="BP45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5846,6 +5911,7 @@
       <c r="BM46" t="inlineStr"/>
       <c r="BN46" t="inlineStr"/>
       <c r="BO46" t="inlineStr"/>
+      <c r="BP46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5935,6 +6001,7 @@
       <c r="BM47" t="inlineStr"/>
       <c r="BN47" t="inlineStr"/>
       <c r="BO47" t="inlineStr"/>
+      <c r="BP47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6016,6 +6083,7 @@
       <c r="BM48" t="inlineStr"/>
       <c r="BN48" t="inlineStr"/>
       <c r="BO48" t="inlineStr"/>
+      <c r="BP48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-06 15:27:24
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BP48"/>
+  <dimension ref="A1:BR48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,6 +772,16 @@
       <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-05</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-06</t>
         </is>
       </c>
     </row>
@@ -852,6 +862,8 @@
       <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -954,6 +966,8 @@
       <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1044,6 +1058,8 @@
       <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1130,6 +1146,8 @@
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1224,6 +1242,8 @@
       <c r="BN6" t="inlineStr"/>
       <c r="BO6" t="inlineStr"/>
       <c r="BP6" t="inlineStr"/>
+      <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1310,6 +1330,8 @@
       <c r="BN7" t="inlineStr"/>
       <c r="BO7" t="inlineStr"/>
       <c r="BP7" t="inlineStr"/>
+      <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1400,6 +1422,8 @@
       <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="inlineStr"/>
       <c r="BP8" t="inlineStr"/>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1486,6 +1510,8 @@
       <c r="BN9" t="inlineStr"/>
       <c r="BO9" t="inlineStr"/>
       <c r="BP9" t="inlineStr"/>
+      <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1791,7 +1817,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP10" t="inlineStr"/>
+      <c r="BP10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2046,6 +2078,8 @@
       </c>
       <c r="BO11" t="inlineStr"/>
       <c r="BP11" t="inlineStr"/>
+      <c r="BQ11" t="inlineStr"/>
+      <c r="BR11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2208,6 +2242,8 @@
       <c r="BN12" t="inlineStr"/>
       <c r="BO12" t="inlineStr"/>
       <c r="BP12" t="inlineStr"/>
+      <c r="BQ12" t="inlineStr"/>
+      <c r="BR12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2394,6 +2430,8 @@
       <c r="BN13" t="inlineStr"/>
       <c r="BO13" t="inlineStr"/>
       <c r="BP13" t="inlineStr"/>
+      <c r="BQ13" t="inlineStr"/>
+      <c r="BR13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2488,6 +2526,8 @@
       <c r="BN14" t="inlineStr"/>
       <c r="BO14" t="inlineStr"/>
       <c r="BP14" t="inlineStr"/>
+      <c r="BQ14" t="inlineStr"/>
+      <c r="BR14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2578,6 +2618,8 @@
       <c r="BN15" t="inlineStr"/>
       <c r="BO15" t="inlineStr"/>
       <c r="BP15" t="inlineStr"/>
+      <c r="BQ15" t="inlineStr"/>
+      <c r="BR15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2696,6 +2738,8 @@
       <c r="BN16" t="inlineStr"/>
       <c r="BO16" t="inlineStr"/>
       <c r="BP16" t="inlineStr"/>
+      <c r="BQ16" t="inlineStr"/>
+      <c r="BR16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2786,6 +2830,12 @@
       <c r="BN17" t="inlineStr"/>
       <c r="BO17" t="inlineStr"/>
       <c r="BP17" t="inlineStr"/>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2868,6 +2918,8 @@
       <c r="BN18" t="inlineStr"/>
       <c r="BO18" t="inlineStr"/>
       <c r="BP18" t="inlineStr"/>
+      <c r="BQ18" t="inlineStr"/>
+      <c r="BR18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2978,6 +3030,12 @@
       <c r="BN19" t="inlineStr"/>
       <c r="BO19" t="inlineStr"/>
       <c r="BP19" t="inlineStr"/>
+      <c r="BQ19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3112,6 +3170,8 @@
       <c r="BN20" t="inlineStr"/>
       <c r="BO20" t="inlineStr"/>
       <c r="BP20" t="inlineStr"/>
+      <c r="BQ20" t="inlineStr"/>
+      <c r="BR20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3194,6 +3254,8 @@
       <c r="BN21" t="inlineStr"/>
       <c r="BO21" t="inlineStr"/>
       <c r="BP21" t="inlineStr"/>
+      <c r="BQ21" t="inlineStr"/>
+      <c r="BR21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3304,6 +3366,8 @@
       <c r="BN22" t="inlineStr"/>
       <c r="BO22" t="inlineStr"/>
       <c r="BP22" t="inlineStr"/>
+      <c r="BQ22" t="inlineStr"/>
+      <c r="BR22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3426,6 +3490,8 @@
       <c r="BN23" t="inlineStr"/>
       <c r="BO23" t="inlineStr"/>
       <c r="BP23" t="inlineStr"/>
+      <c r="BQ23" t="inlineStr"/>
+      <c r="BR23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3544,6 +3610,8 @@
       </c>
       <c r="BO24" t="inlineStr"/>
       <c r="BP24" t="inlineStr"/>
+      <c r="BQ24" t="inlineStr"/>
+      <c r="BR24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3658,6 +3726,8 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BQ25" t="inlineStr"/>
+      <c r="BR25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3779,7 +3849,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP26" t="inlineStr"/>
+      <c r="BP26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3878,6 +3958,8 @@
       <c r="BN27" t="inlineStr"/>
       <c r="BO27" t="inlineStr"/>
       <c r="BP27" t="inlineStr"/>
+      <c r="BQ27" t="inlineStr"/>
+      <c r="BR27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3960,6 +4042,8 @@
       <c r="BN28" t="inlineStr"/>
       <c r="BO28" t="inlineStr"/>
       <c r="BP28" t="inlineStr"/>
+      <c r="BQ28" t="inlineStr"/>
+      <c r="BR28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4066,6 +4150,8 @@
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
+      <c r="BQ29" t="inlineStr"/>
+      <c r="BR29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4164,6 +4250,8 @@
       <c r="BN30" t="inlineStr"/>
       <c r="BO30" t="inlineStr"/>
       <c r="BP30" t="inlineStr"/>
+      <c r="BQ30" t="inlineStr"/>
+      <c r="BR30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4269,7 +4357,17 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BP31" t="inlineStr"/>
+      <c r="BP31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ31" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4387,7 +4485,13 @@
         </is>
       </c>
       <c r="BO32" t="inlineStr"/>
-      <c r="BP32" t="inlineStr"/>
+      <c r="BP32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ32" t="inlineStr"/>
+      <c r="BR32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4470,6 +4574,8 @@
       <c r="BN33" t="inlineStr"/>
       <c r="BO33" t="inlineStr"/>
       <c r="BP33" t="inlineStr"/>
+      <c r="BQ33" t="inlineStr"/>
+      <c r="BR33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4552,6 +4658,8 @@
       <c r="BN34" t="inlineStr"/>
       <c r="BO34" t="inlineStr"/>
       <c r="BP34" t="inlineStr"/>
+      <c r="BQ34" t="inlineStr"/>
+      <c r="BR34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4693,7 +4801,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP35" t="inlineStr"/>
+      <c r="BP35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ35" t="inlineStr"/>
+      <c r="BR35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4812,6 +4926,8 @@
       <c r="BN36" t="inlineStr"/>
       <c r="BO36" t="inlineStr"/>
       <c r="BP36" t="inlineStr"/>
+      <c r="BQ36" t="inlineStr"/>
+      <c r="BR36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4942,6 +5058,8 @@
       <c r="BN37" t="inlineStr"/>
       <c r="BO37" t="inlineStr"/>
       <c r="BP37" t="inlineStr"/>
+      <c r="BQ37" t="inlineStr"/>
+      <c r="BR37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5024,6 +5142,8 @@
       <c r="BN38" t="inlineStr"/>
       <c r="BO38" t="inlineStr"/>
       <c r="BP38" t="inlineStr"/>
+      <c r="BQ38" t="inlineStr"/>
+      <c r="BR38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5134,6 +5254,8 @@
       <c r="BN39" t="inlineStr"/>
       <c r="BO39" t="inlineStr"/>
       <c r="BP39" t="inlineStr"/>
+      <c r="BQ39" t="inlineStr"/>
+      <c r="BR39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5232,6 +5354,8 @@
       <c r="BN40" t="inlineStr"/>
       <c r="BO40" t="inlineStr"/>
       <c r="BP40" t="inlineStr"/>
+      <c r="BQ40" t="inlineStr"/>
+      <c r="BR40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5334,6 +5458,8 @@
       <c r="BN41" t="inlineStr"/>
       <c r="BO41" t="inlineStr"/>
       <c r="BP41" t="inlineStr"/>
+      <c r="BQ41" t="inlineStr"/>
+      <c r="BR41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5463,7 +5589,21 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BP42" t="inlineStr"/>
+      <c r="BP42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5593,7 +5733,21 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP43" t="inlineStr"/>
+      <c r="BP43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5716,6 +5870,8 @@
         </is>
       </c>
       <c r="BP44" t="inlineStr"/>
+      <c r="BQ44" t="inlineStr"/>
+      <c r="BR44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5829,7 +5985,13 @@
         </is>
       </c>
       <c r="BO45" t="inlineStr"/>
-      <c r="BP45" t="inlineStr"/>
+      <c r="BP45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ45" t="inlineStr"/>
+      <c r="BR45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5912,6 +6074,8 @@
       <c r="BN46" t="inlineStr"/>
       <c r="BO46" t="inlineStr"/>
       <c r="BP46" t="inlineStr"/>
+      <c r="BQ46" t="inlineStr"/>
+      <c r="BR46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6002,6 +6166,8 @@
       <c r="BN47" t="inlineStr"/>
       <c r="BO47" t="inlineStr"/>
       <c r="BP47" t="inlineStr"/>
+      <c r="BQ47" t="inlineStr"/>
+      <c r="BR47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6084,6 +6250,8 @@
       <c r="BN48" t="inlineStr"/>
       <c r="BO48" t="inlineStr"/>
       <c r="BP48" t="inlineStr"/>
+      <c r="BQ48" t="inlineStr"/>
+      <c r="BR48" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-09 11:15:15
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BP48"/>
+  <dimension ref="A1:BU49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,6 +772,31 @@
       <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-05</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-06</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-07</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
         </is>
       </c>
     </row>
@@ -852,6 +877,11 @@
       <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -954,6 +984,19 @@
       <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1044,6 +1087,11 @@
       <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1130,6 +1178,11 @@
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
+      <c r="BS5" t="inlineStr"/>
+      <c r="BT5" t="inlineStr"/>
+      <c r="BU5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1224,6 +1277,15 @@
       <c r="BN6" t="inlineStr"/>
       <c r="BO6" t="inlineStr"/>
       <c r="BP6" t="inlineStr"/>
+      <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="inlineStr"/>
+      <c r="BS6" t="inlineStr"/>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>대화 (111.0kg)</t>
+        </is>
+      </c>
+      <c r="BU6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1310,6 +1372,11 @@
       <c r="BN7" t="inlineStr"/>
       <c r="BO7" t="inlineStr"/>
       <c r="BP7" t="inlineStr"/>
+      <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="inlineStr"/>
+      <c r="BS7" t="inlineStr"/>
+      <c r="BT7" t="inlineStr"/>
+      <c r="BU7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1400,6 +1467,11 @@
       <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="inlineStr"/>
       <c r="BP8" t="inlineStr"/>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
+      <c r="BS8" t="inlineStr"/>
+      <c r="BT8" t="inlineStr"/>
+      <c r="BU8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1486,6 +1558,11 @@
       <c r="BN9" t="inlineStr"/>
       <c r="BO9" t="inlineStr"/>
       <c r="BP9" t="inlineStr"/>
+      <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="inlineStr"/>
+      <c r="BS9" t="inlineStr"/>
+      <c r="BT9" t="inlineStr"/>
+      <c r="BU9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1791,7 +1868,28 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP10" t="inlineStr"/>
+      <c r="BP10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BT10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2046,6 +2144,23 @@
       </c>
       <c r="BO11" t="inlineStr"/>
       <c r="BP11" t="inlineStr"/>
+      <c r="BQ11" t="inlineStr"/>
+      <c r="BR11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2208,6 +2323,23 @@
       <c r="BN12" t="inlineStr"/>
       <c r="BO12" t="inlineStr"/>
       <c r="BP12" t="inlineStr"/>
+      <c r="BQ12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS12" t="inlineStr"/>
+      <c r="BT12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2394,6 +2526,19 @@
       <c r="BN13" t="inlineStr"/>
       <c r="BO13" t="inlineStr"/>
       <c r="BP13" t="inlineStr"/>
+      <c r="BQ13" t="inlineStr"/>
+      <c r="BR13" t="inlineStr"/>
+      <c r="BS13" t="inlineStr"/>
+      <c r="BT13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2488,6 +2633,11 @@
       <c r="BN14" t="inlineStr"/>
       <c r="BO14" t="inlineStr"/>
       <c r="BP14" t="inlineStr"/>
+      <c r="BQ14" t="inlineStr"/>
+      <c r="BR14" t="inlineStr"/>
+      <c r="BS14" t="inlineStr"/>
+      <c r="BT14" t="inlineStr"/>
+      <c r="BU14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2578,6 +2728,11 @@
       <c r="BN15" t="inlineStr"/>
       <c r="BO15" t="inlineStr"/>
       <c r="BP15" t="inlineStr"/>
+      <c r="BQ15" t="inlineStr"/>
+      <c r="BR15" t="inlineStr"/>
+      <c r="BS15" t="inlineStr"/>
+      <c r="BT15" t="inlineStr"/>
+      <c r="BU15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2696,6 +2851,11 @@
       <c r="BN16" t="inlineStr"/>
       <c r="BO16" t="inlineStr"/>
       <c r="BP16" t="inlineStr"/>
+      <c r="BQ16" t="inlineStr"/>
+      <c r="BR16" t="inlineStr"/>
+      <c r="BS16" t="inlineStr"/>
+      <c r="BT16" t="inlineStr"/>
+      <c r="BU16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2786,6 +2946,19 @@
       <c r="BN17" t="inlineStr"/>
       <c r="BO17" t="inlineStr"/>
       <c r="BP17" t="inlineStr"/>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr"/>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT17" t="inlineStr"/>
+      <c r="BU17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2868,6 +3041,11 @@
       <c r="BN18" t="inlineStr"/>
       <c r="BO18" t="inlineStr"/>
       <c r="BP18" t="inlineStr"/>
+      <c r="BQ18" t="inlineStr"/>
+      <c r="BR18" t="inlineStr"/>
+      <c r="BS18" t="inlineStr"/>
+      <c r="BT18" t="inlineStr"/>
+      <c r="BU18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2978,6 +3156,27 @@
       <c r="BN19" t="inlineStr"/>
       <c r="BO19" t="inlineStr"/>
       <c r="BP19" t="inlineStr"/>
+      <c r="BQ19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3112,6 +3311,11 @@
       <c r="BN20" t="inlineStr"/>
       <c r="BO20" t="inlineStr"/>
       <c r="BP20" t="inlineStr"/>
+      <c r="BQ20" t="inlineStr"/>
+      <c r="BR20" t="inlineStr"/>
+      <c r="BS20" t="inlineStr"/>
+      <c r="BT20" t="inlineStr"/>
+      <c r="BU20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3194,6 +3398,11 @@
       <c r="BN21" t="inlineStr"/>
       <c r="BO21" t="inlineStr"/>
       <c r="BP21" t="inlineStr"/>
+      <c r="BQ21" t="inlineStr"/>
+      <c r="BR21" t="inlineStr"/>
+      <c r="BS21" t="inlineStr"/>
+      <c r="BT21" t="inlineStr"/>
+      <c r="BU21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3304,6 +3513,15 @@
       <c r="BN22" t="inlineStr"/>
       <c r="BO22" t="inlineStr"/>
       <c r="BP22" t="inlineStr"/>
+      <c r="BQ22" t="inlineStr"/>
+      <c r="BR22" t="inlineStr"/>
+      <c r="BS22" t="inlineStr"/>
+      <c r="BT22" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3426,6 +3644,11 @@
       <c r="BN23" t="inlineStr"/>
       <c r="BO23" t="inlineStr"/>
       <c r="BP23" t="inlineStr"/>
+      <c r="BQ23" t="inlineStr"/>
+      <c r="BR23" t="inlineStr"/>
+      <c r="BS23" t="inlineStr"/>
+      <c r="BT23" t="inlineStr"/>
+      <c r="BU23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3544,6 +3767,19 @@
       </c>
       <c r="BO24" t="inlineStr"/>
       <c r="BP24" t="inlineStr"/>
+      <c r="BQ24" t="inlineStr"/>
+      <c r="BR24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS24" t="inlineStr"/>
+      <c r="BT24" t="inlineStr">
+        <is>
+          <t>대화 (101.0kg)</t>
+        </is>
+      </c>
+      <c r="BU24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3658,6 +3894,15 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BQ25" t="inlineStr"/>
+      <c r="BR25" t="inlineStr"/>
+      <c r="BS25" t="inlineStr"/>
+      <c r="BT25" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3779,7 +4024,28 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP26" t="inlineStr"/>
+      <c r="BP26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS26" t="inlineStr"/>
+      <c r="BT26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3878,6 +4144,11 @@
       <c r="BN27" t="inlineStr"/>
       <c r="BO27" t="inlineStr"/>
       <c r="BP27" t="inlineStr"/>
+      <c r="BQ27" t="inlineStr"/>
+      <c r="BR27" t="inlineStr"/>
+      <c r="BS27" t="inlineStr"/>
+      <c r="BT27" t="inlineStr"/>
+      <c r="BU27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3960,6 +4231,11 @@
       <c r="BN28" t="inlineStr"/>
       <c r="BO28" t="inlineStr"/>
       <c r="BP28" t="inlineStr"/>
+      <c r="BQ28" t="inlineStr"/>
+      <c r="BR28" t="inlineStr"/>
+      <c r="BS28" t="inlineStr"/>
+      <c r="BT28" t="inlineStr"/>
+      <c r="BU28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4066,6 +4342,11 @@
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
+      <c r="BQ29" t="inlineStr"/>
+      <c r="BR29" t="inlineStr"/>
+      <c r="BS29" t="inlineStr"/>
+      <c r="BT29" t="inlineStr"/>
+      <c r="BU29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4164,6 +4445,19 @@
       <c r="BN30" t="inlineStr"/>
       <c r="BO30" t="inlineStr"/>
       <c r="BP30" t="inlineStr"/>
+      <c r="BQ30" t="inlineStr"/>
+      <c r="BR30" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BS30" t="inlineStr"/>
+      <c r="BT30" t="inlineStr">
+        <is>
+          <t>대화 (120.0kg)</t>
+        </is>
+      </c>
+      <c r="BU30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4269,7 +4563,32 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BP31" t="inlineStr"/>
+      <c r="BP31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ31" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BS31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BT31" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4387,7 +4706,20 @@
         </is>
       </c>
       <c r="BO32" t="inlineStr"/>
-      <c r="BP32" t="inlineStr"/>
+      <c r="BP32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ32" t="inlineStr"/>
+      <c r="BR32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS32" t="inlineStr"/>
+      <c r="BT32" t="inlineStr"/>
+      <c r="BU32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4470,6 +4802,11 @@
       <c r="BN33" t="inlineStr"/>
       <c r="BO33" t="inlineStr"/>
       <c r="BP33" t="inlineStr"/>
+      <c r="BQ33" t="inlineStr"/>
+      <c r="BR33" t="inlineStr"/>
+      <c r="BS33" t="inlineStr"/>
+      <c r="BT33" t="inlineStr"/>
+      <c r="BU33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4552,6 +4889,11 @@
       <c r="BN34" t="inlineStr"/>
       <c r="BO34" t="inlineStr"/>
       <c r="BP34" t="inlineStr"/>
+      <c r="BQ34" t="inlineStr"/>
+      <c r="BR34" t="inlineStr"/>
+      <c r="BS34" t="inlineStr"/>
+      <c r="BT34" t="inlineStr"/>
+      <c r="BU34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4693,7 +5035,24 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP35" t="inlineStr"/>
+      <c r="BP35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ35" t="inlineStr"/>
+      <c r="BR35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT35" t="inlineStr"/>
+      <c r="BU35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4812,6 +5171,11 @@
       <c r="BN36" t="inlineStr"/>
       <c r="BO36" t="inlineStr"/>
       <c r="BP36" t="inlineStr"/>
+      <c r="BQ36" t="inlineStr"/>
+      <c r="BR36" t="inlineStr"/>
+      <c r="BS36" t="inlineStr"/>
+      <c r="BT36" t="inlineStr"/>
+      <c r="BU36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4942,6 +5306,23 @@
       <c r="BN37" t="inlineStr"/>
       <c r="BO37" t="inlineStr"/>
       <c r="BP37" t="inlineStr"/>
+      <c r="BQ37" t="inlineStr"/>
+      <c r="BR37" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BS37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT37" t="inlineStr">
+        <is>
+          <t>대화 (79.0kg)</t>
+        </is>
+      </c>
+      <c r="BU37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5024,6 +5405,11 @@
       <c r="BN38" t="inlineStr"/>
       <c r="BO38" t="inlineStr"/>
       <c r="BP38" t="inlineStr"/>
+      <c r="BQ38" t="inlineStr"/>
+      <c r="BR38" t="inlineStr"/>
+      <c r="BS38" t="inlineStr"/>
+      <c r="BT38" t="inlineStr"/>
+      <c r="BU38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5134,6 +5520,11 @@
       <c r="BN39" t="inlineStr"/>
       <c r="BO39" t="inlineStr"/>
       <c r="BP39" t="inlineStr"/>
+      <c r="BQ39" t="inlineStr"/>
+      <c r="BR39" t="inlineStr"/>
+      <c r="BS39" t="inlineStr"/>
+      <c r="BT39" t="inlineStr"/>
+      <c r="BU39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5232,6 +5623,11 @@
       <c r="BN40" t="inlineStr"/>
       <c r="BO40" t="inlineStr"/>
       <c r="BP40" t="inlineStr"/>
+      <c r="BQ40" t="inlineStr"/>
+      <c r="BR40" t="inlineStr"/>
+      <c r="BS40" t="inlineStr"/>
+      <c r="BT40" t="inlineStr"/>
+      <c r="BU40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5334,6 +5730,15 @@
       <c r="BN41" t="inlineStr"/>
       <c r="BO41" t="inlineStr"/>
       <c r="BP41" t="inlineStr"/>
+      <c r="BQ41" t="inlineStr"/>
+      <c r="BR41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS41" t="inlineStr"/>
+      <c r="BT41" t="inlineStr"/>
+      <c r="BU41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5463,7 +5868,36 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BP42" t="inlineStr"/>
+      <c r="BP42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BQ42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BS42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT42" t="inlineStr">
+        <is>
+          <t>대화 (97.0kg)</t>
+        </is>
+      </c>
+      <c r="BU42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5593,7 +6027,36 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BP43" t="inlineStr"/>
+      <c r="BP43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BR43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5716,6 +6179,15 @@
         </is>
       </c>
       <c r="BP44" t="inlineStr"/>
+      <c r="BQ44" t="inlineStr"/>
+      <c r="BR44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS44" t="inlineStr"/>
+      <c r="BT44" t="inlineStr"/>
+      <c r="BU44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5829,7 +6301,20 @@
         </is>
       </c>
       <c r="BO45" t="inlineStr"/>
-      <c r="BP45" t="inlineStr"/>
+      <c r="BP45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ45" t="inlineStr"/>
+      <c r="BR45" t="inlineStr"/>
+      <c r="BS45" t="inlineStr"/>
+      <c r="BT45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5912,6 +6397,11 @@
       <c r="BN46" t="inlineStr"/>
       <c r="BO46" t="inlineStr"/>
       <c r="BP46" t="inlineStr"/>
+      <c r="BQ46" t="inlineStr"/>
+      <c r="BR46" t="inlineStr"/>
+      <c r="BS46" t="inlineStr"/>
+      <c r="BT46" t="inlineStr"/>
+      <c r="BU46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6002,6 +6492,11 @@
       <c r="BN47" t="inlineStr"/>
       <c r="BO47" t="inlineStr"/>
       <c r="BP47" t="inlineStr"/>
+      <c r="BQ47" t="inlineStr"/>
+      <c r="BR47" t="inlineStr"/>
+      <c r="BS47" t="inlineStr"/>
+      <c r="BT47" t="inlineStr"/>
+      <c r="BU47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6084,6 +6579,134 @@
       <c r="BN48" t="inlineStr"/>
       <c r="BO48" t="inlineStr"/>
       <c r="BP48" t="inlineStr"/>
+      <c r="BQ48" t="inlineStr"/>
+      <c r="BR48" t="inlineStr"/>
+      <c r="BS48" t="inlineStr"/>
+      <c r="BT48" t="inlineStr"/>
+      <c r="BU48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>구도원</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>gudowon01</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
+      <c r="Z49" t="inlineStr"/>
+      <c r="AA49" t="inlineStr"/>
+      <c r="AB49" t="inlineStr"/>
+      <c r="AC49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
+      <c r="AI49" t="inlineStr"/>
+      <c r="AJ49" t="inlineStr"/>
+      <c r="AK49" t="inlineStr"/>
+      <c r="AL49" t="inlineStr"/>
+      <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr"/>
+      <c r="AO49" t="inlineStr"/>
+      <c r="AP49" t="inlineStr"/>
+      <c r="AQ49" t="inlineStr"/>
+      <c r="AR49" t="inlineStr"/>
+      <c r="AS49" t="inlineStr"/>
+      <c r="AT49" t="inlineStr"/>
+      <c r="AU49" t="inlineStr"/>
+      <c r="AV49" t="inlineStr"/>
+      <c r="AW49" t="inlineStr"/>
+      <c r="AX49" t="inlineStr"/>
+      <c r="AY49" t="inlineStr"/>
+      <c r="AZ49" t="inlineStr"/>
+      <c r="BA49" t="inlineStr"/>
+      <c r="BB49" t="inlineStr"/>
+      <c r="BC49" t="inlineStr"/>
+      <c r="BD49" t="inlineStr"/>
+      <c r="BE49" t="inlineStr"/>
+      <c r="BF49" t="inlineStr"/>
+      <c r="BG49" t="inlineStr"/>
+      <c r="BH49" t="inlineStr"/>
+      <c r="BI49" t="inlineStr"/>
+      <c r="BJ49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BK49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BL49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BM49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BN49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BO49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BP49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BQ49" t="inlineStr"/>
+      <c r="BR49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BS49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BT49" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BU49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-11 08:01:44
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BU49"/>
+  <dimension ref="A1:BW49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,6 +797,16 @@
       <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-11</t>
         </is>
       </c>
     </row>
@@ -882,6 +892,8 @@
       <c r="BS2" t="inlineStr"/>
       <c r="BT2" t="inlineStr"/>
       <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -997,6 +1009,8 @@
         </is>
       </c>
       <c r="BU3" t="inlineStr"/>
+      <c r="BV3" t="inlineStr"/>
+      <c r="BW3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1092,6 +1106,8 @@
       <c r="BS4" t="inlineStr"/>
       <c r="BT4" t="inlineStr"/>
       <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1183,6 +1199,8 @@
       <c r="BS5" t="inlineStr"/>
       <c r="BT5" t="inlineStr"/>
       <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
+      <c r="BW5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1286,6 +1304,8 @@
         </is>
       </c>
       <c r="BU6" t="inlineStr"/>
+      <c r="BV6" t="inlineStr"/>
+      <c r="BW6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1377,6 +1397,8 @@
       <c r="BS7" t="inlineStr"/>
       <c r="BT7" t="inlineStr"/>
       <c r="BU7" t="inlineStr"/>
+      <c r="BV7" t="inlineStr"/>
+      <c r="BW7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1472,6 +1494,8 @@
       <c r="BS8" t="inlineStr"/>
       <c r="BT8" t="inlineStr"/>
       <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
+      <c r="BW8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1563,6 +1587,8 @@
       <c r="BS9" t="inlineStr"/>
       <c r="BT9" t="inlineStr"/>
       <c r="BU9" t="inlineStr"/>
+      <c r="BV9" t="inlineStr"/>
+      <c r="BW9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1890,6 +1916,12 @@
         </is>
       </c>
       <c r="BU10" t="inlineStr"/>
+      <c r="BV10" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BW10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2161,6 +2193,8 @@
         </is>
       </c>
       <c r="BU11" t="inlineStr"/>
+      <c r="BV11" t="inlineStr"/>
+      <c r="BW11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2340,6 +2374,8 @@
         </is>
       </c>
       <c r="BU12" t="inlineStr"/>
+      <c r="BV12" t="inlineStr"/>
+      <c r="BW12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2539,6 +2575,8 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BV13" t="inlineStr"/>
+      <c r="BW13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2638,6 +2676,8 @@
       <c r="BS14" t="inlineStr"/>
       <c r="BT14" t="inlineStr"/>
       <c r="BU14" t="inlineStr"/>
+      <c r="BV14" t="inlineStr"/>
+      <c r="BW14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2733,6 +2773,8 @@
       <c r="BS15" t="inlineStr"/>
       <c r="BT15" t="inlineStr"/>
       <c r="BU15" t="inlineStr"/>
+      <c r="BV15" t="inlineStr"/>
+      <c r="BW15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2856,6 +2898,8 @@
       <c r="BS16" t="inlineStr"/>
       <c r="BT16" t="inlineStr"/>
       <c r="BU16" t="inlineStr"/>
+      <c r="BV16" t="inlineStr"/>
+      <c r="BW16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2958,7 +3002,17 @@
         </is>
       </c>
       <c r="BT17" t="inlineStr"/>
-      <c r="BU17" t="inlineStr"/>
+      <c r="BU17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3046,6 +3100,8 @@
       <c r="BS18" t="inlineStr"/>
       <c r="BT18" t="inlineStr"/>
       <c r="BU18" t="inlineStr"/>
+      <c r="BV18" t="inlineStr"/>
+      <c r="BW18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3176,7 +3232,21 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BU19" t="inlineStr"/>
+      <c r="BU19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3316,6 +3386,8 @@
       <c r="BS20" t="inlineStr"/>
       <c r="BT20" t="inlineStr"/>
       <c r="BU20" t="inlineStr"/>
+      <c r="BV20" t="inlineStr"/>
+      <c r="BW20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3403,6 +3475,8 @@
       <c r="BS21" t="inlineStr"/>
       <c r="BT21" t="inlineStr"/>
       <c r="BU21" t="inlineStr"/>
+      <c r="BV21" t="inlineStr"/>
+      <c r="BW21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3522,6 +3596,8 @@
         </is>
       </c>
       <c r="BU22" t="inlineStr"/>
+      <c r="BV22" t="inlineStr"/>
+      <c r="BW22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3649,6 +3725,8 @@
       <c r="BS23" t="inlineStr"/>
       <c r="BT23" t="inlineStr"/>
       <c r="BU23" t="inlineStr"/>
+      <c r="BV23" t="inlineStr"/>
+      <c r="BW23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3780,6 +3858,12 @@
         </is>
       </c>
       <c r="BU24" t="inlineStr"/>
+      <c r="BV24" t="inlineStr"/>
+      <c r="BW24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3902,7 +3986,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BU25" t="inlineStr"/>
+      <c r="BU25" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV25" t="inlineStr"/>
+      <c r="BW25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4045,7 +4135,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BU26" t="inlineStr"/>
+      <c r="BU26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV26" t="inlineStr"/>
+      <c r="BW26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4148,7 +4244,21 @@
       <c r="BR27" t="inlineStr"/>
       <c r="BS27" t="inlineStr"/>
       <c r="BT27" t="inlineStr"/>
-      <c r="BU27" t="inlineStr"/>
+      <c r="BU27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4236,6 +4346,8 @@
       <c r="BS28" t="inlineStr"/>
       <c r="BT28" t="inlineStr"/>
       <c r="BU28" t="inlineStr"/>
+      <c r="BV28" t="inlineStr"/>
+      <c r="BW28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4347,6 +4459,8 @@
       <c r="BS29" t="inlineStr"/>
       <c r="BT29" t="inlineStr"/>
       <c r="BU29" t="inlineStr"/>
+      <c r="BV29" t="inlineStr"/>
+      <c r="BW29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4458,6 +4572,8 @@
         </is>
       </c>
       <c r="BU30" t="inlineStr"/>
+      <c r="BV30" t="inlineStr"/>
+      <c r="BW30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4588,7 +4704,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BU31" t="inlineStr"/>
+      <c r="BU31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BV31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BW31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4720,6 +4846,12 @@
       <c r="BS32" t="inlineStr"/>
       <c r="BT32" t="inlineStr"/>
       <c r="BU32" t="inlineStr"/>
+      <c r="BV32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4807,6 +4939,8 @@
       <c r="BS33" t="inlineStr"/>
       <c r="BT33" t="inlineStr"/>
       <c r="BU33" t="inlineStr"/>
+      <c r="BV33" t="inlineStr"/>
+      <c r="BW33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4894,6 +5028,8 @@
       <c r="BS34" t="inlineStr"/>
       <c r="BT34" t="inlineStr"/>
       <c r="BU34" t="inlineStr"/>
+      <c r="BV34" t="inlineStr"/>
+      <c r="BW34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5053,6 +5189,8 @@
       </c>
       <c r="BT35" t="inlineStr"/>
       <c r="BU35" t="inlineStr"/>
+      <c r="BV35" t="inlineStr"/>
+      <c r="BW35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5176,6 +5314,8 @@
       <c r="BS36" t="inlineStr"/>
       <c r="BT36" t="inlineStr"/>
       <c r="BU36" t="inlineStr"/>
+      <c r="BV36" t="inlineStr"/>
+      <c r="BW36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5323,6 +5463,8 @@
         </is>
       </c>
       <c r="BU37" t="inlineStr"/>
+      <c r="BV37" t="inlineStr"/>
+      <c r="BW37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5410,6 +5552,8 @@
       <c r="BS38" t="inlineStr"/>
       <c r="BT38" t="inlineStr"/>
       <c r="BU38" t="inlineStr"/>
+      <c r="BV38" t="inlineStr"/>
+      <c r="BW38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5525,6 +5669,8 @@
       <c r="BS39" t="inlineStr"/>
       <c r="BT39" t="inlineStr"/>
       <c r="BU39" t="inlineStr"/>
+      <c r="BV39" t="inlineStr"/>
+      <c r="BW39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5628,6 +5774,8 @@
       <c r="BS40" t="inlineStr"/>
       <c r="BT40" t="inlineStr"/>
       <c r="BU40" t="inlineStr"/>
+      <c r="BV40" t="inlineStr"/>
+      <c r="BW40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5739,6 +5887,8 @@
       <c r="BS41" t="inlineStr"/>
       <c r="BT41" t="inlineStr"/>
       <c r="BU41" t="inlineStr"/>
+      <c r="BV41" t="inlineStr"/>
+      <c r="BW41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5895,9 +6045,15 @@
       </c>
       <c r="BU42" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BV42" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BW42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6057,6 +6213,12 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BV43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6188,6 +6350,8 @@
       <c r="BS44" t="inlineStr"/>
       <c r="BT44" t="inlineStr"/>
       <c r="BU44" t="inlineStr"/>
+      <c r="BV44" t="inlineStr"/>
+      <c r="BW44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6315,6 +6479,8 @@
         </is>
       </c>
       <c r="BU45" t="inlineStr"/>
+      <c r="BV45" t="inlineStr"/>
+      <c r="BW45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6402,6 +6568,8 @@
       <c r="BS46" t="inlineStr"/>
       <c r="BT46" t="inlineStr"/>
       <c r="BU46" t="inlineStr"/>
+      <c r="BV46" t="inlineStr"/>
+      <c r="BW46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6497,6 +6665,8 @@
       <c r="BS47" t="inlineStr"/>
       <c r="BT47" t="inlineStr"/>
       <c r="BU47" t="inlineStr"/>
+      <c r="BV47" t="inlineStr"/>
+      <c r="BW47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6584,6 +6754,8 @@
       <c r="BS48" t="inlineStr"/>
       <c r="BT48" t="inlineStr"/>
       <c r="BU48" t="inlineStr"/>
+      <c r="BV48" t="inlineStr"/>
+      <c r="BW48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6707,6 +6879,8 @@
         </is>
       </c>
       <c r="BU49" t="inlineStr"/>
+      <c r="BV49" t="inlineStr"/>
+      <c r="BW49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
6/9조한범 문호현 추가 ## 분석 시간: 2025-06-11 17:18:45
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW49"/>
+  <dimension ref="A1:BW51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1921,7 +1921,11 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BW10" t="inlineStr"/>
+      <c r="BW10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2375,7 +2379,11 @@
       </c>
       <c r="BU12" t="inlineStr"/>
       <c r="BV12" t="inlineStr"/>
-      <c r="BW12" t="inlineStr"/>
+      <c r="BW12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2575,8 +2583,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BV13" t="inlineStr"/>
-      <c r="BW13" t="inlineStr"/>
+      <c r="BV13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4141,7 +4157,11 @@
         </is>
       </c>
       <c r="BV26" t="inlineStr"/>
-      <c r="BW26" t="inlineStr"/>
+      <c r="BW26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5315,7 +5335,11 @@
       <c r="BT36" t="inlineStr"/>
       <c r="BU36" t="inlineStr"/>
       <c r="BV36" t="inlineStr"/>
-      <c r="BW36" t="inlineStr"/>
+      <c r="BW36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5463,8 +5487,16 @@
         </is>
       </c>
       <c r="BU37" t="inlineStr"/>
-      <c r="BV37" t="inlineStr"/>
-      <c r="BW37" t="inlineStr"/>
+      <c r="BV37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW37" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -6053,7 +6085,11 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BW42" t="inlineStr"/>
+      <c r="BW42" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6218,7 +6254,11 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BW43" t="inlineStr"/>
+      <c r="BW43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6882,6 +6922,180 @@
       <c r="BV49" t="inlineStr"/>
       <c r="BW49" t="inlineStr"/>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>조한범</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>jiangel79ki1024</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
+      <c r="AB50" t="inlineStr"/>
+      <c r="AC50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
+      <c r="AI50" t="inlineStr"/>
+      <c r="AJ50" t="inlineStr"/>
+      <c r="AK50" t="inlineStr"/>
+      <c r="AL50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr"/>
+      <c r="AO50" t="inlineStr"/>
+      <c r="AP50" t="inlineStr"/>
+      <c r="AQ50" t="inlineStr"/>
+      <c r="AR50" t="inlineStr"/>
+      <c r="AS50" t="inlineStr"/>
+      <c r="AT50" t="inlineStr"/>
+      <c r="AU50" t="inlineStr"/>
+      <c r="AV50" t="inlineStr"/>
+      <c r="AW50" t="inlineStr"/>
+      <c r="AX50" t="inlineStr"/>
+      <c r="AY50" t="inlineStr"/>
+      <c r="AZ50" t="inlineStr"/>
+      <c r="BA50" t="inlineStr"/>
+      <c r="BB50" t="inlineStr"/>
+      <c r="BC50" t="inlineStr"/>
+      <c r="BD50" t="inlineStr"/>
+      <c r="BE50" t="inlineStr"/>
+      <c r="BF50" t="inlineStr"/>
+      <c r="BG50" t="inlineStr"/>
+      <c r="BH50" t="inlineStr"/>
+      <c r="BI50" t="inlineStr"/>
+      <c r="BJ50" t="inlineStr"/>
+      <c r="BK50" t="inlineStr"/>
+      <c r="BL50" t="inlineStr"/>
+      <c r="BM50" t="inlineStr"/>
+      <c r="BN50" t="inlineStr"/>
+      <c r="BO50" t="inlineStr"/>
+      <c r="BP50" t="inlineStr"/>
+      <c r="BQ50" t="inlineStr"/>
+      <c r="BR50" t="inlineStr"/>
+      <c r="BS50" t="inlineStr"/>
+      <c r="BT50" t="inlineStr"/>
+      <c r="BU50" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BV50" t="inlineStr"/>
+      <c r="BW50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Monhohyeon080306</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Monhohyeon080306</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
+      <c r="AB51" t="inlineStr"/>
+      <c r="AC51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
+      <c r="AI51" t="inlineStr"/>
+      <c r="AJ51" t="inlineStr"/>
+      <c r="AK51" t="inlineStr"/>
+      <c r="AL51" t="inlineStr"/>
+      <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr"/>
+      <c r="AO51" t="inlineStr"/>
+      <c r="AP51" t="inlineStr"/>
+      <c r="AQ51" t="inlineStr"/>
+      <c r="AR51" t="inlineStr"/>
+      <c r="AS51" t="inlineStr"/>
+      <c r="AT51" t="inlineStr"/>
+      <c r="AU51" t="inlineStr"/>
+      <c r="AV51" t="inlineStr"/>
+      <c r="AW51" t="inlineStr"/>
+      <c r="AX51" t="inlineStr"/>
+      <c r="AY51" t="inlineStr"/>
+      <c r="AZ51" t="inlineStr"/>
+      <c r="BA51" t="inlineStr"/>
+      <c r="BB51" t="inlineStr"/>
+      <c r="BC51" t="inlineStr"/>
+      <c r="BD51" t="inlineStr"/>
+      <c r="BE51" t="inlineStr"/>
+      <c r="BF51" t="inlineStr"/>
+      <c r="BG51" t="inlineStr"/>
+      <c r="BH51" t="inlineStr"/>
+      <c r="BI51" t="inlineStr"/>
+      <c r="BJ51" t="inlineStr"/>
+      <c r="BK51" t="inlineStr"/>
+      <c r="BL51" t="inlineStr"/>
+      <c r="BM51" t="inlineStr"/>
+      <c r="BN51" t="inlineStr"/>
+      <c r="BO51" t="inlineStr"/>
+      <c r="BP51" t="inlineStr"/>
+      <c r="BQ51" t="inlineStr"/>
+      <c r="BR51" t="inlineStr"/>
+      <c r="BS51" t="inlineStr"/>
+      <c r="BT51" t="inlineStr"/>
+      <c r="BU51" t="inlineStr"/>
+      <c r="BV51" t="inlineStr"/>
+      <c r="BW51" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
분석 시간: 2025-06-12 08:36:24
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW51"/>
+  <dimension ref="A1:BX51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,11 @@
       <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>2025-06-11</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-12</t>
         </is>
       </c>
     </row>
@@ -894,6 +899,7 @@
       <c r="BU2" t="inlineStr"/>
       <c r="BV2" t="inlineStr"/>
       <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1011,6 +1017,7 @@
       <c r="BU3" t="inlineStr"/>
       <c r="BV3" t="inlineStr"/>
       <c r="BW3" t="inlineStr"/>
+      <c r="BX3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1108,6 +1115,7 @@
       <c r="BU4" t="inlineStr"/>
       <c r="BV4" t="inlineStr"/>
       <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1201,6 +1209,7 @@
       <c r="BU5" t="inlineStr"/>
       <c r="BV5" t="inlineStr"/>
       <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1306,6 +1315,7 @@
       <c r="BU6" t="inlineStr"/>
       <c r="BV6" t="inlineStr"/>
       <c r="BW6" t="inlineStr"/>
+      <c r="BX6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1399,6 +1409,7 @@
       <c r="BU7" t="inlineStr"/>
       <c r="BV7" t="inlineStr"/>
       <c r="BW7" t="inlineStr"/>
+      <c r="BX7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1496,6 +1507,7 @@
       <c r="BU8" t="inlineStr"/>
       <c r="BV8" t="inlineStr"/>
       <c r="BW8" t="inlineStr"/>
+      <c r="BX8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1589,6 +1601,7 @@
       <c r="BU9" t="inlineStr"/>
       <c r="BV9" t="inlineStr"/>
       <c r="BW9" t="inlineStr"/>
+      <c r="BX9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1926,6 +1939,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2199,6 +2213,7 @@
       <c r="BU11" t="inlineStr"/>
       <c r="BV11" t="inlineStr"/>
       <c r="BW11" t="inlineStr"/>
+      <c r="BX11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2384,6 +2399,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2593,6 +2609,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2694,6 +2711,7 @@
       <c r="BU14" t="inlineStr"/>
       <c r="BV14" t="inlineStr"/>
       <c r="BW14" t="inlineStr"/>
+      <c r="BX14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2791,6 +2809,7 @@
       <c r="BU15" t="inlineStr"/>
       <c r="BV15" t="inlineStr"/>
       <c r="BW15" t="inlineStr"/>
+      <c r="BX15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2916,6 +2935,7 @@
       <c r="BU16" t="inlineStr"/>
       <c r="BV16" t="inlineStr"/>
       <c r="BW16" t="inlineStr"/>
+      <c r="BX16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3028,7 +3048,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BW17" t="inlineStr"/>
+      <c r="BW17" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BX17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3118,6 +3143,7 @@
       <c r="BU18" t="inlineStr"/>
       <c r="BV18" t="inlineStr"/>
       <c r="BW18" t="inlineStr"/>
+      <c r="BX18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3263,6 +3289,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3404,6 +3431,7 @@
       <c r="BU20" t="inlineStr"/>
       <c r="BV20" t="inlineStr"/>
       <c r="BW20" t="inlineStr"/>
+      <c r="BX20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3493,6 +3521,7 @@
       <c r="BU21" t="inlineStr"/>
       <c r="BV21" t="inlineStr"/>
       <c r="BW21" t="inlineStr"/>
+      <c r="BX21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3613,7 +3642,12 @@
       </c>
       <c r="BU22" t="inlineStr"/>
       <c r="BV22" t="inlineStr"/>
-      <c r="BW22" t="inlineStr"/>
+      <c r="BW22" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BX22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3743,6 +3777,7 @@
       <c r="BU23" t="inlineStr"/>
       <c r="BV23" t="inlineStr"/>
       <c r="BW23" t="inlineStr"/>
+      <c r="BX23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3880,6 +3915,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4009,6 +4045,7 @@
       </c>
       <c r="BV25" t="inlineStr"/>
       <c r="BW25" t="inlineStr"/>
+      <c r="BX25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4162,6 +4199,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4279,6 +4317,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4368,6 +4407,7 @@
       <c r="BU28" t="inlineStr"/>
       <c r="BV28" t="inlineStr"/>
       <c r="BW28" t="inlineStr"/>
+      <c r="BX28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4481,6 +4521,7 @@
       <c r="BU29" t="inlineStr"/>
       <c r="BV29" t="inlineStr"/>
       <c r="BW29" t="inlineStr"/>
+      <c r="BX29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4594,6 +4635,7 @@
       <c r="BU30" t="inlineStr"/>
       <c r="BV30" t="inlineStr"/>
       <c r="BW30" t="inlineStr"/>
+      <c r="BX30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4734,7 +4776,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BW31" t="inlineStr"/>
+      <c r="BW31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BX31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4872,6 +4919,7 @@
         </is>
       </c>
       <c r="BW32" t="inlineStr"/>
+      <c r="BX32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4961,6 +5009,7 @@
       <c r="BU33" t="inlineStr"/>
       <c r="BV33" t="inlineStr"/>
       <c r="BW33" t="inlineStr"/>
+      <c r="BX33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5050,6 +5099,7 @@
       <c r="BU34" t="inlineStr"/>
       <c r="BV34" t="inlineStr"/>
       <c r="BW34" t="inlineStr"/>
+      <c r="BX34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5210,7 +5260,12 @@
       <c r="BT35" t="inlineStr"/>
       <c r="BU35" t="inlineStr"/>
       <c r="BV35" t="inlineStr"/>
-      <c r="BW35" t="inlineStr"/>
+      <c r="BW35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BX35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5340,6 +5395,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5497,6 +5553,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5586,6 +5643,7 @@
       <c r="BU38" t="inlineStr"/>
       <c r="BV38" t="inlineStr"/>
       <c r="BW38" t="inlineStr"/>
+      <c r="BX38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5703,6 +5761,7 @@
       <c r="BU39" t="inlineStr"/>
       <c r="BV39" t="inlineStr"/>
       <c r="BW39" t="inlineStr"/>
+      <c r="BX39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5808,6 +5867,7 @@
       <c r="BU40" t="inlineStr"/>
       <c r="BV40" t="inlineStr"/>
       <c r="BW40" t="inlineStr"/>
+      <c r="BX40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5920,7 +5980,12 @@
       <c r="BT41" t="inlineStr"/>
       <c r="BU41" t="inlineStr"/>
       <c r="BV41" t="inlineStr"/>
-      <c r="BW41" t="inlineStr"/>
+      <c r="BW41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BX41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6087,6 +6152,11 @@
       </c>
       <c r="BW42" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="BX42" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -6259,6 +6329,7 @@
           <t>식단</t>
         </is>
       </c>
+      <c r="BX43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6392,6 +6463,7 @@
       <c r="BU44" t="inlineStr"/>
       <c r="BV44" t="inlineStr"/>
       <c r="BW44" t="inlineStr"/>
+      <c r="BX44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6519,8 +6591,17 @@
         </is>
       </c>
       <c r="BU45" t="inlineStr"/>
-      <c r="BV45" t="inlineStr"/>
-      <c r="BW45" t="inlineStr"/>
+      <c r="BV45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BW45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="BX45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6610,6 +6691,7 @@
       <c r="BU46" t="inlineStr"/>
       <c r="BV46" t="inlineStr"/>
       <c r="BW46" t="inlineStr"/>
+      <c r="BX46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6707,6 +6789,7 @@
       <c r="BU47" t="inlineStr"/>
       <c r="BV47" t="inlineStr"/>
       <c r="BW47" t="inlineStr"/>
+      <c r="BX47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6796,6 +6879,7 @@
       <c r="BU48" t="inlineStr"/>
       <c r="BV48" t="inlineStr"/>
       <c r="BW48" t="inlineStr"/>
+      <c r="BX48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6921,6 +7005,7 @@
       <c r="BU49" t="inlineStr"/>
       <c r="BV49" t="inlineStr"/>
       <c r="BW49" t="inlineStr"/>
+      <c r="BX49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7010,6 +7095,7 @@
       </c>
       <c r="BV50" t="inlineStr"/>
       <c r="BW50" t="inlineStr"/>
+      <c r="BX50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -7095,6 +7181,7 @@
       <c r="BU51" t="inlineStr"/>
       <c r="BV51" t="inlineStr"/>
       <c r="BW51" t="inlineStr"/>
+      <c r="BX51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-16 10:55:22
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BZ51"/>
+  <dimension ref="A1:CB51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -822,6 +822,16 @@
       <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-15</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
         </is>
       </c>
     </row>
@@ -912,6 +922,8 @@
       <c r="BX2" t="inlineStr"/>
       <c r="BY2" t="inlineStr"/>
       <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1031,7 +1043,13 @@
       <c r="BW3" t="inlineStr"/>
       <c r="BX3" t="inlineStr"/>
       <c r="BY3" t="inlineStr"/>
-      <c r="BZ3" t="inlineStr"/>
+      <c r="BZ3" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA3" t="inlineStr"/>
+      <c r="CB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1132,6 +1150,8 @@
       <c r="BX4" t="inlineStr"/>
       <c r="BY4" t="inlineStr"/>
       <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1228,6 +1248,8 @@
       <c r="BX5" t="inlineStr"/>
       <c r="BY5" t="inlineStr"/>
       <c r="BZ5" t="inlineStr"/>
+      <c r="CA5" t="inlineStr"/>
+      <c r="CB5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1340,6 +1362,8 @@
       </c>
       <c r="BY6" t="inlineStr"/>
       <c r="BZ6" t="inlineStr"/>
+      <c r="CA6" t="inlineStr"/>
+      <c r="CB6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1436,6 +1460,8 @@
       <c r="BX7" t="inlineStr"/>
       <c r="BY7" t="inlineStr"/>
       <c r="BZ7" t="inlineStr"/>
+      <c r="CA7" t="inlineStr"/>
+      <c r="CB7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1543,7 +1569,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BZ8" t="inlineStr"/>
+      <c r="BZ8" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA8" t="inlineStr"/>
+      <c r="CB8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1640,6 +1672,12 @@
       <c r="BX9" t="inlineStr"/>
       <c r="BY9" t="inlineStr"/>
       <c r="BZ9" t="inlineStr"/>
+      <c r="CA9" t="inlineStr"/>
+      <c r="CB9" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1988,6 +2026,12 @@
         </is>
       </c>
       <c r="BZ10" t="inlineStr"/>
+      <c r="CA10" t="inlineStr">
+        <is>
+          <t>대화 (79.7kg)</t>
+        </is>
+      </c>
+      <c r="CB10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2271,7 +2315,21 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BZ11" t="inlineStr"/>
+      <c r="BZ11" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CA11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB11" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2459,7 +2517,13 @@
       </c>
       <c r="BX12" t="inlineStr"/>
       <c r="BY12" t="inlineStr"/>
-      <c r="BZ12" t="inlineStr"/>
+      <c r="BZ12" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA12" t="inlineStr"/>
+      <c r="CB12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2676,6 +2740,12 @@
       </c>
       <c r="BY13" t="inlineStr"/>
       <c r="BZ13" t="inlineStr"/>
+      <c r="CA13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2780,6 +2850,8 @@
       <c r="BX14" t="inlineStr"/>
       <c r="BY14" t="inlineStr"/>
       <c r="BZ14" t="inlineStr"/>
+      <c r="CA14" t="inlineStr"/>
+      <c r="CB14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2880,6 +2952,8 @@
       <c r="BX15" t="inlineStr"/>
       <c r="BY15" t="inlineStr"/>
       <c r="BZ15" t="inlineStr"/>
+      <c r="CA15" t="inlineStr"/>
+      <c r="CB15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3008,6 +3082,8 @@
       <c r="BX16" t="inlineStr"/>
       <c r="BY16" t="inlineStr"/>
       <c r="BZ16" t="inlineStr"/>
+      <c r="CA16" t="inlineStr"/>
+      <c r="CB16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3128,6 +3204,8 @@
       <c r="BX17" t="inlineStr"/>
       <c r="BY17" t="inlineStr"/>
       <c r="BZ17" t="inlineStr"/>
+      <c r="CA17" t="inlineStr"/>
+      <c r="CB17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3220,6 +3298,8 @@
       <c r="BX18" t="inlineStr"/>
       <c r="BY18" t="inlineStr"/>
       <c r="BZ18" t="inlineStr"/>
+      <c r="CA18" t="inlineStr"/>
+      <c r="CB18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3375,7 +3455,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BZ19" t="inlineStr"/>
+      <c r="BZ19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3520,6 +3610,8 @@
       <c r="BX20" t="inlineStr"/>
       <c r="BY20" t="inlineStr"/>
       <c r="BZ20" t="inlineStr"/>
+      <c r="CA20" t="inlineStr"/>
+      <c r="CB20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3612,6 +3704,8 @@
       <c r="BX21" t="inlineStr"/>
       <c r="BY21" t="inlineStr"/>
       <c r="BZ21" t="inlineStr"/>
+      <c r="CA21" t="inlineStr"/>
+      <c r="CB21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3744,6 +3838,8 @@
         </is>
       </c>
       <c r="BZ22" t="inlineStr"/>
+      <c r="CA22" t="inlineStr"/>
+      <c r="CB22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3876,6 +3972,8 @@
       <c r="BX23" t="inlineStr"/>
       <c r="BY23" t="inlineStr"/>
       <c r="BZ23" t="inlineStr"/>
+      <c r="CA23" t="inlineStr"/>
+      <c r="CB23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4020,6 +4118,12 @@
       </c>
       <c r="BY24" t="inlineStr"/>
       <c r="BZ24" t="inlineStr"/>
+      <c r="CA24" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4152,6 +4256,8 @@
       <c r="BX25" t="inlineStr"/>
       <c r="BY25" t="inlineStr"/>
       <c r="BZ25" t="inlineStr"/>
+      <c r="CA25" t="inlineStr"/>
+      <c r="CB25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4308,6 +4414,8 @@
       <c r="BX26" t="inlineStr"/>
       <c r="BY26" t="inlineStr"/>
       <c r="BZ26" t="inlineStr"/>
+      <c r="CA26" t="inlineStr"/>
+      <c r="CB26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4428,6 +4536,12 @@
       <c r="BX27" t="inlineStr"/>
       <c r="BY27" t="inlineStr"/>
       <c r="BZ27" t="inlineStr"/>
+      <c r="CA27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4520,6 +4634,8 @@
       <c r="BX28" t="inlineStr"/>
       <c r="BY28" t="inlineStr"/>
       <c r="BZ28" t="inlineStr"/>
+      <c r="CA28" t="inlineStr"/>
+      <c r="CB28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4636,6 +4752,8 @@
       <c r="BX29" t="inlineStr"/>
       <c r="BY29" t="inlineStr"/>
       <c r="BZ29" t="inlineStr"/>
+      <c r="CA29" t="inlineStr"/>
+      <c r="CB29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4752,6 +4870,8 @@
       <c r="BX30" t="inlineStr"/>
       <c r="BY30" t="inlineStr"/>
       <c r="BZ30" t="inlineStr"/>
+      <c r="CA30" t="inlineStr"/>
+      <c r="CB30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4907,7 +5027,17 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="BZ31" t="inlineStr"/>
+      <c r="BZ31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CA31" t="inlineStr">
+        <is>
+          <t>대화 (72.9kg)</t>
+        </is>
+      </c>
+      <c r="CB31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -5051,7 +5181,13 @@
         </is>
       </c>
       <c r="BY32" t="inlineStr"/>
-      <c r="BZ32" t="inlineStr"/>
+      <c r="BZ32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA32" t="inlineStr"/>
+      <c r="CB32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5144,6 +5280,8 @@
       <c r="BX33" t="inlineStr"/>
       <c r="BY33" t="inlineStr"/>
       <c r="BZ33" t="inlineStr"/>
+      <c r="CA33" t="inlineStr"/>
+      <c r="CB33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5236,6 +5374,8 @@
       <c r="BX34" t="inlineStr"/>
       <c r="BY34" t="inlineStr"/>
       <c r="BZ34" t="inlineStr"/>
+      <c r="CA34" t="inlineStr"/>
+      <c r="CB34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5411,7 +5551,13 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BZ35" t="inlineStr"/>
+      <c r="BZ35" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA35" t="inlineStr"/>
+      <c r="CB35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5544,6 +5690,8 @@
       <c r="BX36" t="inlineStr"/>
       <c r="BY36" t="inlineStr"/>
       <c r="BZ36" t="inlineStr"/>
+      <c r="CA36" t="inlineStr"/>
+      <c r="CB36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5709,9 +5857,15 @@
       <c r="BY37" t="inlineStr"/>
       <c r="BZ37" t="inlineStr">
         <is>
-          <t>식단</t>
-        </is>
-      </c>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CA37" t="inlineStr">
+        <is>
+          <t>대화 (78.9kg)</t>
+        </is>
+      </c>
+      <c r="CB37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5804,6 +5958,8 @@
       <c r="BX38" t="inlineStr"/>
       <c r="BY38" t="inlineStr"/>
       <c r="BZ38" t="inlineStr"/>
+      <c r="CA38" t="inlineStr"/>
+      <c r="CB38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5924,6 +6080,8 @@
       <c r="BX39" t="inlineStr"/>
       <c r="BY39" t="inlineStr"/>
       <c r="BZ39" t="inlineStr"/>
+      <c r="CA39" t="inlineStr"/>
+      <c r="CB39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6032,6 +6190,8 @@
       <c r="BX40" t="inlineStr"/>
       <c r="BY40" t="inlineStr"/>
       <c r="BZ40" t="inlineStr"/>
+      <c r="CA40" t="inlineStr"/>
+      <c r="CB40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6156,6 +6316,8 @@
       </c>
       <c r="BY41" t="inlineStr"/>
       <c r="BZ41" t="inlineStr"/>
+      <c r="CA41" t="inlineStr"/>
+      <c r="CB41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6337,6 +6499,16 @@
       </c>
       <c r="BZ42" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CA42" t="inlineStr">
+        <is>
+          <t>대화 (97.7kg)</t>
+        </is>
+      </c>
+      <c r="CB42" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -6519,7 +6691,21 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="BZ43" t="inlineStr"/>
+      <c r="BZ43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CA43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB43" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6660,6 +6846,8 @@
         </is>
       </c>
       <c r="BZ44" t="inlineStr"/>
+      <c r="CA44" t="inlineStr"/>
+      <c r="CB44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6804,6 +6992,12 @@
       </c>
       <c r="BY45" t="inlineStr"/>
       <c r="BZ45" t="inlineStr"/>
+      <c r="CA45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6896,6 +7090,8 @@
       <c r="BX46" t="inlineStr"/>
       <c r="BY46" t="inlineStr"/>
       <c r="BZ46" t="inlineStr"/>
+      <c r="CA46" t="inlineStr"/>
+      <c r="CB46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6996,6 +7192,8 @@
       <c r="BX47" t="inlineStr"/>
       <c r="BY47" t="inlineStr"/>
       <c r="BZ47" t="inlineStr"/>
+      <c r="CA47" t="inlineStr"/>
+      <c r="CB47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7088,6 +7286,8 @@
       <c r="BX48" t="inlineStr"/>
       <c r="BY48" t="inlineStr"/>
       <c r="BZ48" t="inlineStr"/>
+      <c r="CA48" t="inlineStr"/>
+      <c r="CB48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -7220,6 +7420,8 @@
       </c>
       <c r="BY49" t="inlineStr"/>
       <c r="BZ49" t="inlineStr"/>
+      <c r="CA49" t="inlineStr"/>
+      <c r="CB49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7312,6 +7514,8 @@
       <c r="BX50" t="inlineStr"/>
       <c r="BY50" t="inlineStr"/>
       <c r="BZ50" t="inlineStr"/>
+      <c r="CA50" t="inlineStr"/>
+      <c r="CB50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -7400,6 +7604,8 @@
       <c r="BX51" t="inlineStr"/>
       <c r="BY51" t="inlineStr"/>
       <c r="BZ51" t="inlineStr"/>
+      <c r="CA51" t="inlineStr"/>
+      <c r="CB51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
분석 시간: 2025-06-19 14:25:19
</commit_message>
<xml_diff>
--- a/체다_대화_식단_기록.xlsx
+++ b/체다_대화_식단_기록.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CD51"/>
+  <dimension ref="A1:CE51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -842,6 +842,11 @@
       <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
         </is>
       </c>
     </row>
@@ -936,6 +941,7 @@
       <c r="CB2" t="inlineStr"/>
       <c r="CC2" t="inlineStr"/>
       <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1064,6 +1070,11 @@
       <c r="CB3" t="inlineStr"/>
       <c r="CC3" t="inlineStr"/>
       <c r="CD3" t="inlineStr"/>
+      <c r="CE3" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1168,6 +1179,7 @@
       <c r="CB4" t="inlineStr"/>
       <c r="CC4" t="inlineStr"/>
       <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1268,6 +1280,7 @@
       <c r="CB5" t="inlineStr"/>
       <c r="CC5" t="inlineStr"/>
       <c r="CD5" t="inlineStr"/>
+      <c r="CE5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1384,6 +1397,7 @@
       <c r="CB6" t="inlineStr"/>
       <c r="CC6" t="inlineStr"/>
       <c r="CD6" t="inlineStr"/>
+      <c r="CE6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1484,6 +1498,7 @@
       <c r="CB7" t="inlineStr"/>
       <c r="CC7" t="inlineStr"/>
       <c r="CD7" t="inlineStr"/>
+      <c r="CE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1600,6 +1615,7 @@
       <c r="CB8" t="inlineStr"/>
       <c r="CC8" t="inlineStr"/>
       <c r="CD8" t="inlineStr"/>
+      <c r="CE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1704,6 +1720,7 @@
       </c>
       <c r="CC9" t="inlineStr"/>
       <c r="CD9" t="inlineStr"/>
+      <c r="CE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2063,7 +2080,12 @@
           <t>대화</t>
         </is>
       </c>
-      <c r="CD10" t="inlineStr"/>
+      <c r="CD10" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2368,6 +2390,7 @@
         </is>
       </c>
       <c r="CD11" t="inlineStr"/>
+      <c r="CE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2564,6 +2587,7 @@
       <c r="CB12" t="inlineStr"/>
       <c r="CC12" t="inlineStr"/>
       <c r="CD12" t="inlineStr"/>
+      <c r="CE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2787,7 +2811,12 @@
       </c>
       <c r="CB13" t="inlineStr"/>
       <c r="CC13" t="inlineStr"/>
-      <c r="CD13" t="inlineStr"/>
+      <c r="CD13" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2896,6 +2925,7 @@
       <c r="CB14" t="inlineStr"/>
       <c r="CC14" t="inlineStr"/>
       <c r="CD14" t="inlineStr"/>
+      <c r="CE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3000,6 +3030,7 @@
       <c r="CB15" t="inlineStr"/>
       <c r="CC15" t="inlineStr"/>
       <c r="CD15" t="inlineStr"/>
+      <c r="CE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3132,6 +3163,7 @@
       <c r="CB16" t="inlineStr"/>
       <c r="CC16" t="inlineStr"/>
       <c r="CD16" t="inlineStr"/>
+      <c r="CE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3260,6 +3292,7 @@
       </c>
       <c r="CC17" t="inlineStr"/>
       <c r="CD17" t="inlineStr"/>
+      <c r="CE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3356,6 +3389,7 @@
       <c r="CB18" t="inlineStr"/>
       <c r="CC18" t="inlineStr"/>
       <c r="CD18" t="inlineStr"/>
+      <c r="CE18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3531,7 +3565,16 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="CD19" t="inlineStr"/>
+      <c r="CD19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE19" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3680,6 +3723,7 @@
       <c r="CB20" t="inlineStr"/>
       <c r="CC20" t="inlineStr"/>
       <c r="CD20" t="inlineStr"/>
+      <c r="CE20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3776,6 +3820,7 @@
       <c r="CB21" t="inlineStr"/>
       <c r="CC21" t="inlineStr"/>
       <c r="CD21" t="inlineStr"/>
+      <c r="CE21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3912,6 +3957,7 @@
       <c r="CB22" t="inlineStr"/>
       <c r="CC22" t="inlineStr"/>
       <c r="CD22" t="inlineStr"/>
+      <c r="CE22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -4056,6 +4102,7 @@
         </is>
       </c>
       <c r="CD23" t="inlineStr"/>
+      <c r="CE23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4212,6 +4259,7 @@
       </c>
       <c r="CC24" t="inlineStr"/>
       <c r="CD24" t="inlineStr"/>
+      <c r="CE24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4348,6 +4396,7 @@
       <c r="CB25" t="inlineStr"/>
       <c r="CC25" t="inlineStr"/>
       <c r="CD25" t="inlineStr"/>
+      <c r="CE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4507,7 +4556,12 @@
       <c r="CA26" t="inlineStr"/>
       <c r="CB26" t="inlineStr"/>
       <c r="CC26" t="inlineStr"/>
-      <c r="CD26" t="inlineStr"/>
+      <c r="CD26" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4639,7 +4693,12 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="CD27" t="inlineStr"/>
+      <c r="CD27" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4736,6 +4795,7 @@
       <c r="CB28" t="inlineStr"/>
       <c r="CC28" t="inlineStr"/>
       <c r="CD28" t="inlineStr"/>
+      <c r="CE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4856,6 +4916,7 @@
       <c r="CB29" t="inlineStr"/>
       <c r="CC29" t="inlineStr"/>
       <c r="CD29" t="inlineStr"/>
+      <c r="CE29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4975,7 +5036,12 @@
       <c r="CA30" t="inlineStr"/>
       <c r="CB30" t="inlineStr"/>
       <c r="CC30" t="inlineStr"/>
-      <c r="CD30" t="inlineStr"/>
+      <c r="CD30" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -5143,7 +5209,12 @@
       </c>
       <c r="CB31" t="inlineStr"/>
       <c r="CC31" t="inlineStr"/>
-      <c r="CD31" t="inlineStr"/>
+      <c r="CD31" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CE31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -5295,7 +5366,16 @@
       <c r="CA32" t="inlineStr"/>
       <c r="CB32" t="inlineStr"/>
       <c r="CC32" t="inlineStr"/>
-      <c r="CD32" t="inlineStr"/>
+      <c r="CD32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE32" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5392,6 +5472,7 @@
       <c r="CB33" t="inlineStr"/>
       <c r="CC33" t="inlineStr"/>
       <c r="CD33" t="inlineStr"/>
+      <c r="CE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5488,6 +5569,7 @@
       <c r="CB34" t="inlineStr"/>
       <c r="CC34" t="inlineStr"/>
       <c r="CD34" t="inlineStr"/>
+      <c r="CE34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5672,6 +5754,7 @@
       <c r="CB35" t="inlineStr"/>
       <c r="CC35" t="inlineStr"/>
       <c r="CD35" t="inlineStr"/>
+      <c r="CE35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5807,7 +5890,12 @@
       <c r="CA36" t="inlineStr"/>
       <c r="CB36" t="inlineStr"/>
       <c r="CC36" t="inlineStr"/>
-      <c r="CD36" t="inlineStr"/>
+      <c r="CD36" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5993,6 +6081,11 @@
       </c>
       <c r="CD37" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CE37" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -6092,6 +6185,7 @@
       <c r="CB38" t="inlineStr"/>
       <c r="CC38" t="inlineStr"/>
       <c r="CD38" t="inlineStr"/>
+      <c r="CE38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -6220,6 +6314,7 @@
       </c>
       <c r="CC39" t="inlineStr"/>
       <c r="CD39" t="inlineStr"/>
+      <c r="CE39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6336,6 +6431,7 @@
       </c>
       <c r="CC40" t="inlineStr"/>
       <c r="CD40" t="inlineStr"/>
+      <c r="CE40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6461,9 +6557,22 @@
       <c r="BY41" t="inlineStr"/>
       <c r="BZ41" t="inlineStr"/>
       <c r="CA41" t="inlineStr"/>
-      <c r="CB41" t="inlineStr"/>
-      <c r="CC41" t="inlineStr"/>
-      <c r="CD41" t="inlineStr"/>
+      <c r="CB41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CC41" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CD41" t="inlineStr">
+        <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CE41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6665,6 +6774,11 @@
       </c>
       <c r="CD42" t="inlineStr">
         <is>
+          <t>대화</t>
+        </is>
+      </c>
+      <c r="CE42" t="inlineStr">
+        <is>
           <t>식단</t>
         </is>
       </c>
@@ -6864,6 +6978,7 @@
       </c>
       <c r="CC43" t="inlineStr"/>
       <c r="CD43" t="inlineStr"/>
+      <c r="CE43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -7008,6 +7123,11 @@
       <c r="CB44" t="inlineStr"/>
       <c r="CC44" t="inlineStr"/>
       <c r="CD44" t="inlineStr"/>
+      <c r="CE44" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -7162,8 +7282,17 @@
           <t>식단</t>
         </is>
       </c>
-      <c r="CC45" t="inlineStr"/>
-      <c r="CD45" t="inlineStr"/>
+      <c r="CC45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CD45" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -7260,6 +7389,7 @@
       <c r="CB46" t="inlineStr"/>
       <c r="CC46" t="inlineStr"/>
       <c r="CD46" t="inlineStr"/>
+      <c r="CE46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -7364,6 +7494,7 @@
       <c r="CB47" t="inlineStr"/>
       <c r="CC47" t="inlineStr"/>
       <c r="CD47" t="inlineStr"/>
+      <c r="CE47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7460,6 +7591,7 @@
       <c r="CB48" t="inlineStr"/>
       <c r="CC48" t="inlineStr"/>
       <c r="CD48" t="inlineStr"/>
+      <c r="CE48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -7604,6 +7736,7 @@
         </is>
       </c>
       <c r="CD49" t="inlineStr"/>
+      <c r="CE49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7700,16 +7833,17 @@
       <c r="CB50" t="inlineStr"/>
       <c r="CC50" t="inlineStr"/>
       <c r="CD50" t="inlineStr"/>
+      <c r="CE50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Monhohyeon080306</t>
+          <t>문호현</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Monhohyeon080306</t>
+          <t>monhohyeon080306</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -7782,16 +7916,33 @@
       <c r="BR51" t="inlineStr"/>
       <c r="BS51" t="inlineStr"/>
       <c r="BT51" t="inlineStr"/>
-      <c r="BU51" t="inlineStr"/>
+      <c r="BU51" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
       <c r="BV51" t="inlineStr"/>
       <c r="BW51" t="inlineStr"/>
       <c r="BX51" t="inlineStr"/>
       <c r="BY51" t="inlineStr"/>
       <c r="BZ51" t="inlineStr"/>
-      <c r="CA51" t="inlineStr"/>
-      <c r="CB51" t="inlineStr"/>
+      <c r="CA51" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CB51" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
       <c r="CC51" t="inlineStr"/>
-      <c r="CD51" t="inlineStr"/>
+      <c r="CD51" t="inlineStr">
+        <is>
+          <t>식단</t>
+        </is>
+      </c>
+      <c r="CE51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>